<commit_message>
Added base functionality required for calculating the pipetting dispense height
</commit_message>
<xml_diff>
--- a/Method Maker1.xlsx
+++ b/Method Maker1.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonMethodMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35A21F8C-28B5-4B3B-A9AF-B1EF47FFF630}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958AC26F-F5D6-45EA-AD87-391BE0048A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15750" yWindow="-15870" windowWidth="25440" windowHeight="15390" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="___Dropdown values" sheetId="4" r:id="rId1"/>
     <sheet name="Building Blocks" sheetId="1" r:id="rId2"/>
     <sheet name="Method" sheetId="2" r:id="rId3"/>
-    <sheet name="Worklist" sheetId="3" r:id="rId4"/>
+    <sheet name="SolutionPrep" sheetId="5" r:id="rId4"/>
+    <sheet name="Worklist" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="87">
   <si>
     <t>Liquid Transfer</t>
   </si>
@@ -273,9 +273,6 @@
     <t>Buffer/Diluent</t>
   </si>
   <si>
-    <t>7M GnHCl in 100mM Tris pH8.2</t>
-  </si>
-  <si>
     <t>Denaturant</t>
   </si>
   <si>
@@ -289,6 +286,18 @@
   </si>
   <si>
     <t>50% TFA</t>
+  </si>
+  <si>
+    <t>1st Pipetting Step</t>
+  </si>
+  <si>
+    <t>Liquid 1</t>
+  </si>
+  <si>
+    <t>Liquid 2</t>
+  </si>
+  <si>
+    <t>Liquid 3</t>
   </si>
 </sst>
 </file>
@@ -760,6 +769,99 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -787,98 +889,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -886,10 +907,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -898,25 +925,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1461,7 +1470,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -1531,31 +1540,31 @@
   <sheetData>
     <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="71"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="81"/>
+      <c r="H3" s="72"/>
       <c r="I3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="84" t="s">
+      <c r="K3" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="85"/>
+      <c r="L3" s="76"/>
       <c r="M3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="78" t="s">
+      <c r="O3" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="79"/>
+      <c r="P3" s="68"/>
       <c r="Q3" s="28" t="s">
         <v>16</v>
       </c>
@@ -1565,74 +1574,74 @@
         <v>1</v>
       </c>
       <c r="D4" s="34"/>
-      <c r="E4" s="72"/>
+      <c r="E4" s="61"/>
       <c r="G4" s="7" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="15"/>
-      <c r="I4" s="95"/>
+      <c r="I4" s="86"/>
       <c r="K4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="L4" s="20"/>
-      <c r="M4" s="98"/>
+      <c r="M4" s="89"/>
       <c r="O4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="P4" s="22"/>
-      <c r="Q4" s="67"/>
+      <c r="Q4" s="98"/>
     </row>
     <row r="5" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="33"/>
-      <c r="E5" s="73"/>
+      <c r="E5" s="62"/>
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="96"/>
+      <c r="I5" s="87"/>
       <c r="K5" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L5" s="20"/>
-      <c r="M5" s="99"/>
+      <c r="M5" s="90"/>
       <c r="O5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="P5" s="22"/>
-      <c r="Q5" s="68"/>
+      <c r="Q5" s="99"/>
     </row>
     <row r="6" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="15"/>
-      <c r="I6" s="96"/>
+      <c r="I6" s="87"/>
       <c r="K6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="L6" s="21"/>
-      <c r="M6" s="100"/>
+      <c r="M6" s="91"/>
       <c r="O6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="P6" s="23"/>
-      <c r="Q6" s="69"/>
+      <c r="Q6" s="100"/>
     </row>
     <row r="7" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="15"/>
-      <c r="I7" s="96"/>
+      <c r="I7" s="87"/>
     </row>
     <row r="8" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="83"/>
+      <c r="D8" s="74"/>
       <c r="E8" s="25" t="s">
         <v>16</v>
       </c>
@@ -1640,25 +1649,25 @@
         <v>11</v>
       </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="97"/>
+      <c r="I8" s="88"/>
     </row>
     <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="86"/>
-      <c r="K9" s="70" t="s">
+      <c r="E9" s="77"/>
+      <c r="K9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="71"/>
+      <c r="L9" s="70"/>
       <c r="M9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="78" t="s">
+      <c r="O9" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="P9" s="79"/>
+      <c r="P9" s="68"/>
       <c r="Q9" s="28" t="s">
         <v>16</v>
       </c>
@@ -1668,11 +1677,11 @@
         <v>38</v>
       </c>
       <c r="D10" s="18"/>
-      <c r="E10" s="87"/>
-      <c r="G10" s="63" t="s">
+      <c r="E10" s="78"/>
+      <c r="G10" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="64"/>
+      <c r="H10" s="95"/>
       <c r="I10" s="29" t="s">
         <v>16</v>
       </c>
@@ -1680,7 +1689,7 @@
         <v>61</v>
       </c>
       <c r="L10" s="32"/>
-      <c r="M10" s="89"/>
+      <c r="M10" s="80"/>
       <c r="O10" s="44" t="s">
         <v>13</v>
       </c>
@@ -1692,42 +1701,42 @@
         <v>39</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="88"/>
+      <c r="E11" s="79"/>
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="13"/>
-      <c r="I11" s="92"/>
+      <c r="I11" s="83"/>
       <c r="K11" s="31" t="s">
         <v>23</v>
       </c>
       <c r="L11" s="32"/>
-      <c r="M11" s="90"/>
+      <c r="M11" s="81"/>
     </row>
     <row r="12" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H12" s="13"/>
-      <c r="I12" s="93"/>
+      <c r="I12" s="84"/>
       <c r="K12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="33"/>
-      <c r="M12" s="91"/>
-      <c r="O12" s="78" t="s">
+      <c r="M12" s="82"/>
+      <c r="O12" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="P12" s="79"/>
+      <c r="P12" s="68"/>
       <c r="Q12" s="28" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="70" t="s">
+      <c r="C13" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="71"/>
+      <c r="D13" s="70"/>
       <c r="E13" s="47" t="s">
         <v>16</v>
       </c>
@@ -1735,7 +1744,7 @@
         <v>64</v>
       </c>
       <c r="H13" s="13"/>
-      <c r="I13" s="93"/>
+      <c r="I13" s="84"/>
       <c r="O13" s="12" t="s">
         <v>9</v>
       </c>
@@ -1743,33 +1752,33 @@
       <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="74"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="72"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="61"/>
       <c r="G14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="13"/>
-      <c r="I14" s="93"/>
+      <c r="I14" s="84"/>
     </row>
     <row r="15" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="76"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="73"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="62"/>
       <c r="G15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="94"/>
+      <c r="I15" s="85"/>
     </row>
     <row r="17" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="96" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="66"/>
+      <c r="H18" s="97"/>
       <c r="I18" s="36" t="s">
         <v>16</v>
       </c>
@@ -1779,17 +1788,22 @@
         <v>50</v>
       </c>
       <c r="H19" s="38"/>
-      <c r="I19" s="61"/>
+      <c r="I19" s="92"/>
     </row>
     <row r="20" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G20" s="39" t="s">
         <v>46</v>
       </c>
       <c r="H20" s="40"/>
-      <c r="I20" s="62"/>
+      <c r="I20" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="K9:L9"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="C14:D15"/>
@@ -1806,11 +1820,6 @@
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1894,8 +1903,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:E19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1907,7 +1916,8 @@
     <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.140625" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.5703125" style="24" customWidth="1"/>
     <col min="15" max="15" width="9.140625" style="24"/>
@@ -1915,10 +1925,10 @@
   <sheetData>
     <row r="1" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="71"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="30" t="s">
         <v>16</v>
       </c>
@@ -1930,7 +1940,7 @@
       <c r="E3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="61" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1941,20 +1951,20 @@
       <c r="E4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="73"/>
+      <c r="F4" s="62"/>
     </row>
     <row r="6" spans="4:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="109" t="s">
+      <c r="D6" s="113" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="109"/>
+      <c r="E6" s="113"/>
     </row>
     <row r="7" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="107" t="s">
+      <c r="D8" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="108"/>
+      <c r="E8" s="102"/>
       <c r="F8" s="41" t="s">
         <v>16</v>
       </c>
@@ -1966,7 +1976,7 @@
       <c r="E9" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="105"/>
+      <c r="F9" s="111"/>
     </row>
     <row r="10" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
@@ -1975,7 +1985,7 @@
       <c r="E10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="106"/>
+      <c r="F10" s="112"/>
     </row>
     <row r="11" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I11" s="24"/>
@@ -1998,10 +2008,11 @@
       <c r="D13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="92"/>
+      <c r="E13" s="13" t="str">
+        <f>Worklist!G1</f>
+        <v>1st Pipetting Step</v>
+      </c>
+      <c r="F13" s="83"/>
       <c r="N13"/>
       <c r="O13"/>
     </row>
@@ -2010,9 +2021,9 @@
         <v>66</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="F14" s="93"/>
+        <v>78</v>
+      </c>
+      <c r="F14" s="84"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="N14"/>
@@ -2025,7 +2036,7 @@
       <c r="E15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="93"/>
+      <c r="F15" s="84"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="N15"/>
@@ -2038,7 +2049,7 @@
       <c r="E16" s="13">
         <v>600</v>
       </c>
-      <c r="F16" s="93"/>
+      <c r="F16" s="84"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="N16"/>
@@ -2051,7 +2062,7 @@
       <c r="E17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="94"/>
+      <c r="F17" s="85"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="N17"/>
@@ -2064,10 +2075,10 @@
       <c r="O18"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="81"/>
+      <c r="E19" s="72"/>
       <c r="F19" s="26" t="s">
         <v>16</v>
       </c>
@@ -2083,7 +2094,7 @@
       <c r="E20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="95"/>
+      <c r="F20" s="86"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="N20"/>
@@ -2096,7 +2107,7 @@
       <c r="E21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="96"/>
+      <c r="F21" s="87"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="N21"/>
@@ -2110,7 +2121,7 @@
         <f>Worklist!E1</f>
         <v>_Conc</v>
       </c>
-      <c r="F22" s="96"/>
+      <c r="F22" s="87"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="N22"/>
@@ -2123,7 +2134,7 @@
       <c r="E23" s="15">
         <v>10</v>
       </c>
-      <c r="F23" s="96"/>
+      <c r="F23" s="87"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="N23"/>
@@ -2136,7 +2147,7 @@
       <c r="E24" s="16">
         <v>50</v>
       </c>
-      <c r="F24" s="97"/>
+      <c r="F24" s="88"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="N24"/>
@@ -2163,9 +2174,9 @@
         <v>1</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="92"/>
+        <v>79</v>
+      </c>
+      <c r="F28" s="83"/>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D29" s="3" t="s">
@@ -2174,7 +2185,7 @@
       <c r="E29" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="93"/>
+      <c r="F29" s="84"/>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
@@ -2183,7 +2194,7 @@
       <c r="E30" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="93"/>
+      <c r="F30" s="84"/>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D31" s="3" t="s">
@@ -2192,7 +2203,7 @@
       <c r="E31" s="13">
         <v>5</v>
       </c>
-      <c r="F31" s="93"/>
+      <c r="F31" s="84"/>
     </row>
     <row r="32" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="4" t="s">
@@ -2201,14 +2212,14 @@
       <c r="E32" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="94"/>
+      <c r="F32" s="85"/>
     </row>
     <row r="33" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" s="101" t="s">
+      <c r="D34" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="102"/>
+      <c r="E34" s="106"/>
       <c r="F34" s="28" t="s">
         <v>16</v>
       </c>
@@ -2220,7 +2231,7 @@
       <c r="E35" s="22">
         <v>37</v>
       </c>
-      <c r="F35" s="67"/>
+      <c r="F35" s="98"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D36" s="11" t="s">
@@ -2229,7 +2240,7 @@
       <c r="E36" s="22">
         <v>60</v>
       </c>
-      <c r="F36" s="68"/>
+      <c r="F36" s="99"/>
     </row>
     <row r="37" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="12" t="s">
@@ -2238,7 +2249,7 @@
       <c r="E37" s="23">
         <v>0</v>
       </c>
-      <c r="F37" s="69"/>
+      <c r="F37" s="100"/>
     </row>
     <row r="38" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
@@ -2257,7 +2268,7 @@
       <c r="E40" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="92"/>
+      <c r="F40" s="83"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D41" s="3" t="s">
@@ -2266,7 +2277,7 @@
       <c r="E41" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F41" s="93"/>
+      <c r="F41" s="84"/>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D42" s="3" t="s">
@@ -2275,7 +2286,7 @@
       <c r="E42" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="93"/>
+      <c r="F42" s="84"/>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D43" s="3" t="s">
@@ -2284,7 +2295,7 @@
       <c r="E43" s="13">
         <v>6</v>
       </c>
-      <c r="F43" s="93"/>
+      <c r="F43" s="84"/>
     </row>
     <row r="44" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="4" t="s">
@@ -2293,14 +2304,14 @@
       <c r="E44" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="94"/>
+      <c r="F44" s="85"/>
     </row>
     <row r="45" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="101" t="s">
+      <c r="D46" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="102"/>
+      <c r="E46" s="106"/>
       <c r="F46" s="28" t="s">
         <v>16</v>
       </c>
@@ -2312,7 +2323,7 @@
       <c r="E47" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F47" s="67"/>
+      <c r="F47" s="98"/>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D48" s="11" t="s">
@@ -2321,7 +2332,7 @@
       <c r="E48" s="22">
         <v>60</v>
       </c>
-      <c r="F48" s="68"/>
+      <c r="F48" s="99"/>
     </row>
     <row r="49" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="12" t="s">
@@ -2330,14 +2341,14 @@
       <c r="E49" s="23">
         <v>0</v>
       </c>
-      <c r="F49" s="69"/>
+      <c r="F49" s="100"/>
     </row>
     <row r="50" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D51" s="107" t="s">
+      <c r="D51" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="E51" s="108"/>
+      <c r="E51" s="102"/>
       <c r="F51" s="51" t="s">
         <v>16</v>
       </c>
@@ -2347,9 +2358,9 @@
         <v>1</v>
       </c>
       <c r="E52" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="F52" s="72"/>
+        <v>80</v>
+      </c>
+      <c r="F52" s="61"/>
     </row>
     <row r="53" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="1" t="s">
@@ -2358,14 +2369,14 @@
       <c r="E53" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F53" s="73"/>
+      <c r="F53" s="62"/>
     </row>
     <row r="54" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D55" s="110" t="s">
+      <c r="D55" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="111"/>
+      <c r="E55" s="108"/>
       <c r="F55" s="49" t="s">
         <v>16</v>
       </c>
@@ -2377,16 +2388,16 @@
       <c r="E56" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F56" s="98"/>
+      <c r="F56" s="89"/>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D57" s="5" t="s">
         <v>40</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F57" s="99"/>
+        <v>79</v>
+      </c>
+      <c r="F57" s="90"/>
     </row>
     <row r="58" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="6" t="s">
@@ -2395,14 +2406,14 @@
       <c r="E58" s="21">
         <v>300</v>
       </c>
-      <c r="F58" s="100"/>
+      <c r="F58" s="91"/>
     </row>
     <row r="59" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="112" t="s">
+      <c r="D60" s="109" t="s">
         <v>4</v>
       </c>
-      <c r="E60" s="113"/>
+      <c r="E60" s="110"/>
       <c r="F60" s="25" t="s">
         <v>16</v>
       </c>
@@ -2415,7 +2426,7 @@
         <f>Worklist!F1</f>
         <v>Digestion Pathway</v>
       </c>
-      <c r="F61" s="86"/>
+      <c r="F61" s="77"/>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D62" s="9" t="s">
@@ -2424,7 +2435,7 @@
       <c r="E62" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F62" s="87"/>
+      <c r="F62" s="78"/>
     </row>
     <row r="63" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="10" t="s">
@@ -2433,21 +2444,21 @@
       <c r="E63" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F63" s="88"/>
+      <c r="F63" s="79"/>
     </row>
     <row r="64" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="70" t="s">
+      <c r="B65" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="71"/>
+      <c r="C65" s="70"/>
       <c r="D65" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="F65" s="107" t="s">
+      <c r="F65" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="G65" s="108"/>
+      <c r="G65" s="102"/>
       <c r="H65" s="51" t="s">
         <v>16</v>
       </c>
@@ -2459,14 +2470,14 @@
       <c r="C66" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D66" s="72"/>
+      <c r="D66" s="61"/>
       <c r="F66" s="31" t="s">
         <v>1</v>
       </c>
       <c r="G66" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H66" s="72"/>
+      <c r="H66" s="61"/>
     </row>
     <row r="67" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
@@ -2475,14 +2486,14 @@
       <c r="C67" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D67" s="73"/>
+      <c r="D67" s="62"/>
       <c r="F67" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G67" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H67" s="73"/>
+      <c r="H67" s="62"/>
     </row>
     <row r="68" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="24"/>
@@ -2493,10 +2504,10 @@
       <c r="H68" s="57"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="63" t="s">
+      <c r="B69" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="64"/>
+      <c r="C69" s="95"/>
       <c r="D69" s="50" t="s">
         <v>16</v>
       </c>
@@ -2513,16 +2524,16 @@
         <v>1</v>
       </c>
       <c r="C70" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D70" s="92"/>
+        <v>80</v>
+      </c>
+      <c r="D70" s="83"/>
       <c r="F70" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H70" s="92"/>
+        <v>80</v>
+      </c>
+      <c r="H70" s="83"/>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
@@ -2531,14 +2542,14 @@
       <c r="C71" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D71" s="93"/>
+      <c r="D71" s="84"/>
       <c r="F71" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H71" s="93"/>
+      <c r="H71" s="84"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
@@ -2547,14 +2558,14 @@
       <c r="C72" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="93"/>
+      <c r="D72" s="84"/>
       <c r="F72" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H72" s="93"/>
+      <c r="H72" s="84"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
@@ -2563,14 +2574,14 @@
       <c r="C73" s="13">
         <v>250</v>
       </c>
-      <c r="D73" s="93"/>
+      <c r="D73" s="84"/>
       <c r="F73" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G73" s="13">
         <v>250</v>
       </c>
-      <c r="H73" s="93"/>
+      <c r="H73" s="84"/>
     </row>
     <row r="74" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="4" t="s">
@@ -2579,21 +2590,21 @@
       <c r="C74" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D74" s="94"/>
+      <c r="D74" s="85"/>
       <c r="F74" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G74" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H74" s="94"/>
+      <c r="H74" s="85"/>
     </row>
     <row r="75" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="63" t="s">
+      <c r="B76" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="64"/>
+      <c r="C76" s="95"/>
       <c r="D76" s="50" t="s">
         <v>16</v>
       </c>
@@ -2612,14 +2623,14 @@
       <c r="C77" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D77" s="92"/>
+      <c r="D77" s="83"/>
       <c r="F77" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="H77" s="92"/>
+        <v>81</v>
+      </c>
+      <c r="H77" s="83"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
@@ -2628,14 +2639,14 @@
       <c r="C78" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D78" s="93"/>
+      <c r="D78" s="84"/>
       <c r="F78" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H78" s="93"/>
+      <c r="H78" s="84"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
@@ -2644,14 +2655,14 @@
       <c r="C79" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D79" s="93"/>
+      <c r="D79" s="84"/>
       <c r="F79" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="H79" s="93"/>
+      <c r="H79" s="84"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
@@ -2660,14 +2671,14 @@
       <c r="C80" s="13">
         <v>3.6</v>
       </c>
-      <c r="D80" s="93"/>
+      <c r="D80" s="84"/>
       <c r="F80" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G80" s="13">
         <v>30</v>
       </c>
-      <c r="H80" s="93"/>
+      <c r="H80" s="84"/>
     </row>
     <row r="81" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="4" t="s">
@@ -2676,28 +2687,28 @@
       <c r="C81" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D81" s="94"/>
+      <c r="D81" s="85"/>
       <c r="F81" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G81" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H81" s="94"/>
+      <c r="H81" s="85"/>
     </row>
     <row r="82" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="78" t="s">
+      <c r="B83" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="C83" s="79"/>
+      <c r="C83" s="68"/>
       <c r="D83" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F83" s="101" t="s">
+      <c r="F83" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="G83" s="102"/>
+      <c r="G83" s="106"/>
       <c r="H83" s="28" t="s">
         <v>16</v>
       </c>
@@ -2709,14 +2720,14 @@
       <c r="C84" s="22">
         <v>37</v>
       </c>
-      <c r="D84" s="67"/>
+      <c r="D84" s="98"/>
       <c r="F84" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G84" s="22">
         <v>37</v>
       </c>
-      <c r="H84" s="67"/>
+      <c r="H84" s="98"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="11" t="s">
@@ -2726,14 +2737,14 @@
         <f>18*60</f>
         <v>1080</v>
       </c>
-      <c r="D85" s="68"/>
+      <c r="D85" s="99"/>
       <c r="F85" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G85" s="22">
         <v>5000</v>
       </c>
-      <c r="H85" s="68"/>
+      <c r="H85" s="99"/>
     </row>
     <row r="86" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="12" t="s">
@@ -2742,21 +2753,21 @@
       <c r="C86" s="23">
         <v>0</v>
       </c>
-      <c r="D86" s="69"/>
+      <c r="D86" s="100"/>
       <c r="F86" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G86" s="23">
         <v>0</v>
       </c>
-      <c r="H86" s="69"/>
+      <c r="H86" s="100"/>
     </row>
     <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="63" t="s">
+      <c r="B88" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C88" s="64"/>
+      <c r="C88" s="95"/>
       <c r="D88" s="50" t="s">
         <v>16</v>
       </c>
@@ -2773,16 +2784,16 @@
         <v>1</v>
       </c>
       <c r="C89" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D89" s="92"/>
+        <v>81</v>
+      </c>
+      <c r="D89" s="83"/>
       <c r="F89" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H89" s="92"/>
+        <v>82</v>
+      </c>
+      <c r="H89" s="83"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
@@ -2791,14 +2802,14 @@
       <c r="C90" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D90" s="93"/>
+      <c r="D90" s="84"/>
       <c r="F90" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H90" s="93"/>
+      <c r="H90" s="84"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
@@ -2807,14 +2818,14 @@
       <c r="C91" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D91" s="93"/>
+      <c r="D91" s="84"/>
       <c r="F91" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H91" s="93"/>
+      <c r="H91" s="84"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
@@ -2823,14 +2834,14 @@
       <c r="C92" s="55">
         <v>30</v>
       </c>
-      <c r="D92" s="93"/>
+      <c r="D92" s="84"/>
       <c r="F92" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G92" s="13">
         <v>14.2</v>
       </c>
-      <c r="H92" s="93"/>
+      <c r="H92" s="84"/>
     </row>
     <row r="93" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="4" t="s">
@@ -2839,28 +2850,28 @@
       <c r="C93" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D93" s="94"/>
+      <c r="D93" s="85"/>
       <c r="F93" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G93" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H93" s="94"/>
+      <c r="H93" s="85"/>
     </row>
     <row r="94" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="78" t="s">
+      <c r="B95" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="C95" s="79"/>
+      <c r="C95" s="68"/>
       <c r="D95" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F95" s="107" t="s">
+      <c r="F95" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="G95" s="108"/>
+      <c r="G95" s="102"/>
       <c r="H95" s="51" t="s">
         <v>16</v>
       </c>
@@ -2872,10 +2883,10 @@
       <c r="C96" s="22">
         <v>37</v>
       </c>
-      <c r="D96" s="67"/>
-      <c r="F96" s="74"/>
-      <c r="G96" s="75"/>
-      <c r="H96" s="72"/>
+      <c r="D96" s="98"/>
+      <c r="F96" s="63"/>
+      <c r="G96" s="64"/>
+      <c r="H96" s="61"/>
     </row>
     <row r="97" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="11" t="s">
@@ -2885,10 +2896,10 @@
         <f>60*4</f>
         <v>240</v>
       </c>
-      <c r="D97" s="68"/>
-      <c r="F97" s="76"/>
-      <c r="G97" s="77"/>
-      <c r="H97" s="73"/>
+      <c r="D97" s="99"/>
+      <c r="F97" s="65"/>
+      <c r="G97" s="66"/>
+      <c r="H97" s="62"/>
     </row>
     <row r="98" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="12" t="s">
@@ -2897,14 +2908,14 @@
       <c r="C98" s="23">
         <v>0</v>
       </c>
-      <c r="D98" s="69"/>
+      <c r="D98" s="100"/>
     </row>
     <row r="99" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="63" t="s">
+      <c r="B100" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C100" s="64"/>
+      <c r="C100" s="95"/>
       <c r="D100" s="50" t="s">
         <v>16</v>
       </c>
@@ -2914,9 +2925,9 @@
         <v>1</v>
       </c>
       <c r="C101" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D101" s="92"/>
+        <v>82</v>
+      </c>
+      <c r="D101" s="83"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
@@ -2925,7 +2936,7 @@
       <c r="C102" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D102" s="93"/>
+      <c r="D102" s="84"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
@@ -2934,7 +2945,7 @@
       <c r="C103" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D103" s="93"/>
+      <c r="D103" s="84"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
@@ -2943,7 +2954,7 @@
       <c r="C104" s="13">
         <v>14.2</v>
       </c>
-      <c r="D104" s="93"/>
+      <c r="D104" s="84"/>
     </row>
     <row r="105" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="4" t="s">
@@ -2952,27 +2963,27 @@
       <c r="C105" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D105" s="94"/>
+      <c r="D105" s="85"/>
     </row>
     <row r="106" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="107" t="s">
+      <c r="B107" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="C107" s="108"/>
+      <c r="C107" s="102"/>
       <c r="D107" s="58" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B108" s="74"/>
-      <c r="C108" s="75"/>
-      <c r="D108" s="72"/>
+      <c r="B108" s="63"/>
+      <c r="C108" s="64"/>
+      <c r="D108" s="61"/>
     </row>
     <row r="109" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="76"/>
-      <c r="C109" s="77"/>
-      <c r="D109" s="73"/>
+      <c r="B109" s="65"/>
+      <c r="C109" s="66"/>
+      <c r="D109" s="62"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K111" s="24"/>
@@ -3012,31 +3023,19 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="H89:H93"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="H84:H86"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D89:D93"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="F95:G95"/>
-    <mergeCell ref="B108:C109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="F96:G97"/>
-    <mergeCell ref="H96:H97"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D101:D105"/>
-    <mergeCell ref="D96:D98"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D84:D86"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="H77:H81"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="H70:H74"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B65:C65"/>
@@ -3052,19 +3051,31 @@
     <mergeCell ref="F52:F53"/>
     <mergeCell ref="F61:F63"/>
     <mergeCell ref="F40:F44"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F69:G69"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D84:D86"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="H77:H81"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="B108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="F96:G97"/>
+    <mergeCell ref="H96:H97"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D101:D105"/>
+    <mergeCell ref="D96:D98"/>
+    <mergeCell ref="H89:H93"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="H84:H86"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D89:D93"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="F95:G95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3132,12 +3143,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F70090-C34D-4006-BF44-FF3E7D4D54FA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD529AF6-49B7-49B9-A330-C878FB7908FD}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,6 +3171,7 @@
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
     <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
@@ -3157,7 +3181,7 @@
     <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3176,8 +3200,11 @@
       <c r="F1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>ROW(A1)</f>
         <v>1</v>
@@ -3197,8 +3224,11 @@
       <c r="F2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>ROW(A2)</f>
         <v>2</v>
@@ -3219,8 +3249,11 @@
       <c r="F3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>ROW(A3)</f>
         <v>3</v>
@@ -3240,6 +3273,9 @@
       </c>
       <c r="F4" t="s">
         <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -3279,18 +3315,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3517,18 +3553,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46E792D2-13D9-445F-AE7B-CF179A33399C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158388FD-FCB9-4D40-8807-AFB22AE8C172}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158388FD-FCB9-4D40-8807-AFB22AE8C172}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46E792D2-13D9-445F-AE7B-CF179A33399C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Initial Work on Incubation step almost finished. Need to update sequences that are sent to the Hamilton system. Following work completed:Updated incubation and wait module, added loading write function and read to Configuration module
</commit_message>
<xml_diff>
--- a/Method Maker1.xlsx
+++ b/Method Maker1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonMethodMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958AC26F-F5D6-45EA-AD87-391BE0048A33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C9A437-A61C-4C3F-88EB-6CA93637F58D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
+    <workbookView xWindow="7800" yWindow="1695" windowWidth="15300" windowHeight="11055" firstSheet="1" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="___Dropdown values" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Worklist" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -769,6 +770,39 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -793,12 +827,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -862,61 +890,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -925,7 +908,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1540,31 +1541,31 @@
   <sheetData>
     <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="70"/>
+      <c r="D3" s="71"/>
       <c r="E3" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="72"/>
+      <c r="H3" s="81"/>
       <c r="I3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="75" t="s">
+      <c r="K3" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="76"/>
+      <c r="L3" s="85"/>
       <c r="M3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="67" t="s">
+      <c r="O3" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="68"/>
+      <c r="P3" s="79"/>
       <c r="Q3" s="28" t="s">
         <v>16</v>
       </c>
@@ -1574,74 +1575,74 @@
         <v>1</v>
       </c>
       <c r="D4" s="34"/>
-      <c r="E4" s="61"/>
+      <c r="E4" s="72"/>
       <c r="G4" s="7" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="15"/>
-      <c r="I4" s="86"/>
+      <c r="I4" s="95"/>
       <c r="K4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="L4" s="20"/>
-      <c r="M4" s="89"/>
+      <c r="M4" s="98"/>
       <c r="O4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="P4" s="22"/>
-      <c r="Q4" s="98"/>
+      <c r="Q4" s="67"/>
     </row>
     <row r="5" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="33"/>
-      <c r="E5" s="62"/>
+      <c r="E5" s="73"/>
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="87"/>
+      <c r="I5" s="96"/>
       <c r="K5" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L5" s="20"/>
-      <c r="M5" s="90"/>
+      <c r="M5" s="99"/>
       <c r="O5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="P5" s="22"/>
-      <c r="Q5" s="99"/>
+      <c r="Q5" s="68"/>
     </row>
     <row r="6" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="15"/>
-      <c r="I6" s="87"/>
+      <c r="I6" s="96"/>
       <c r="K6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="L6" s="21"/>
-      <c r="M6" s="91"/>
+      <c r="M6" s="100"/>
       <c r="O6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="P6" s="23"/>
-      <c r="Q6" s="100"/>
+      <c r="Q6" s="69"/>
     </row>
     <row r="7" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="15"/>
-      <c r="I7" s="87"/>
+      <c r="I7" s="96"/>
     </row>
     <row r="8" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="82" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="74"/>
+      <c r="D8" s="83"/>
       <c r="E8" s="25" t="s">
         <v>16</v>
       </c>
@@ -1649,25 +1650,25 @@
         <v>11</v>
       </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="88"/>
+      <c r="I8" s="97"/>
     </row>
     <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="77"/>
-      <c r="K9" s="69" t="s">
+      <c r="E9" s="86"/>
+      <c r="K9" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="70"/>
+      <c r="L9" s="71"/>
       <c r="M9" s="48" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="67" t="s">
+      <c r="O9" s="78" t="s">
         <v>57</v>
       </c>
-      <c r="P9" s="68"/>
+      <c r="P9" s="79"/>
       <c r="Q9" s="28" t="s">
         <v>16</v>
       </c>
@@ -1677,11 +1678,11 @@
         <v>38</v>
       </c>
       <c r="D10" s="18"/>
-      <c r="E10" s="78"/>
-      <c r="G10" s="94" t="s">
+      <c r="E10" s="87"/>
+      <c r="G10" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="95"/>
+      <c r="H10" s="64"/>
       <c r="I10" s="29" t="s">
         <v>16</v>
       </c>
@@ -1689,7 +1690,7 @@
         <v>61</v>
       </c>
       <c r="L10" s="32"/>
-      <c r="M10" s="80"/>
+      <c r="M10" s="89"/>
       <c r="O10" s="44" t="s">
         <v>13</v>
       </c>
@@ -1701,42 +1702,42 @@
         <v>39</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="79"/>
+      <c r="E11" s="88"/>
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="13"/>
-      <c r="I11" s="83"/>
+      <c r="I11" s="92"/>
       <c r="K11" s="31" t="s">
         <v>23</v>
       </c>
       <c r="L11" s="32"/>
-      <c r="M11" s="81"/>
+      <c r="M11" s="90"/>
     </row>
     <row r="12" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
         <v>66</v>
       </c>
       <c r="H12" s="13"/>
-      <c r="I12" s="84"/>
+      <c r="I12" s="93"/>
       <c r="K12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="33"/>
-      <c r="M12" s="82"/>
-      <c r="O12" s="67" t="s">
+      <c r="M12" s="91"/>
+      <c r="O12" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="P12" s="68"/>
+      <c r="P12" s="79"/>
       <c r="Q12" s="28" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="69" t="s">
+      <c r="C13" s="70" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="70"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="47" t="s">
         <v>16</v>
       </c>
@@ -1744,7 +1745,7 @@
         <v>64</v>
       </c>
       <c r="H13" s="13"/>
-      <c r="I13" s="84"/>
+      <c r="I13" s="93"/>
       <c r="O13" s="12" t="s">
         <v>9</v>
       </c>
@@ -1752,33 +1753,33 @@
       <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="63"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="61"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="72"/>
       <c r="G14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="13"/>
-      <c r="I14" s="84"/>
+      <c r="I14" s="93"/>
     </row>
     <row r="15" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="65"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="62"/>
+      <c r="C15" s="76"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="73"/>
       <c r="G15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I15" s="85"/>
+      <c r="I15" s="94"/>
     </row>
     <row r="17" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G18" s="96" t="s">
+      <c r="G18" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="97"/>
+      <c r="H18" s="66"/>
       <c r="I18" s="36" t="s">
         <v>16</v>
       </c>
@@ -1788,22 +1789,17 @@
         <v>50</v>
       </c>
       <c r="H19" s="38"/>
-      <c r="I19" s="92"/>
+      <c r="I19" s="61"/>
     </row>
     <row r="20" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G20" s="39" t="s">
         <v>46</v>
       </c>
       <c r="H20" s="40"/>
-      <c r="I20" s="93"/>
+      <c r="I20" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="K9:L9"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="C14:D15"/>
@@ -1820,6 +1816,11 @@
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="O9:P9"/>
     <mergeCell ref="C13:D13"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1903,8 +1904,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="C37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1925,10 +1926,10 @@
   <sheetData>
     <row r="1" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="70"/>
+      <c r="E2" s="71"/>
       <c r="F2" s="30" t="s">
         <v>16</v>
       </c>
@@ -1940,7 +1941,7 @@
       <c r="E3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="61" t="s">
+      <c r="F3" s="72" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1951,20 +1952,20 @@
       <c r="E4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="62"/>
+      <c r="F4" s="73"/>
     </row>
     <row r="6" spans="4:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="113" t="s">
+      <c r="D6" s="109" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="113"/>
+      <c r="E6" s="109"/>
     </row>
     <row r="7" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="101" t="s">
+      <c r="D8" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="102"/>
+      <c r="E8" s="108"/>
       <c r="F8" s="41" t="s">
         <v>16</v>
       </c>
@@ -1976,7 +1977,7 @@
       <c r="E9" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="111"/>
+      <c r="F9" s="105"/>
     </row>
     <row r="10" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
@@ -1985,7 +1986,7 @@
       <c r="E10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="112"/>
+      <c r="F10" s="106"/>
     </row>
     <row r="11" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I11" s="24"/>
@@ -2012,7 +2013,7 @@
         <f>Worklist!G1</f>
         <v>1st Pipetting Step</v>
       </c>
-      <c r="F13" s="83"/>
+      <c r="F13" s="92"/>
       <c r="N13"/>
       <c r="O13"/>
     </row>
@@ -2023,7 +2024,7 @@
       <c r="E14" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="84"/>
+      <c r="F14" s="93"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="N14"/>
@@ -2036,7 +2037,7 @@
       <c r="E15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="84"/>
+      <c r="F15" s="93"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="N15"/>
@@ -2047,9 +2048,9 @@
         <v>12</v>
       </c>
       <c r="E16" s="13">
-        <v>600</v>
-      </c>
-      <c r="F16" s="84"/>
+        <v>60</v>
+      </c>
+      <c r="F16" s="93"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="N16"/>
@@ -2062,7 +2063,7 @@
       <c r="E17" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="85"/>
+      <c r="F17" s="94"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="N17"/>
@@ -2075,10 +2076,10 @@
       <c r="O18"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="71" t="s">
+      <c r="D19" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="72"/>
+      <c r="E19" s="81"/>
       <c r="F19" s="26" t="s">
         <v>16</v>
       </c>
@@ -2094,7 +2095,7 @@
       <c r="E20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="86"/>
+      <c r="F20" s="95"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="N20"/>
@@ -2107,7 +2108,7 @@
       <c r="E21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="87"/>
+      <c r="F21" s="96"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="N21"/>
@@ -2121,7 +2122,7 @@
         <f>Worklist!E1</f>
         <v>_Conc</v>
       </c>
-      <c r="F22" s="87"/>
+      <c r="F22" s="96"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="N22"/>
@@ -2134,7 +2135,7 @@
       <c r="E23" s="15">
         <v>10</v>
       </c>
-      <c r="F23" s="87"/>
+      <c r="F23" s="96"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="N23"/>
@@ -2147,7 +2148,7 @@
       <c r="E24" s="16">
         <v>50</v>
       </c>
-      <c r="F24" s="88"/>
+      <c r="F24" s="97"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="N24"/>
@@ -2176,7 +2177,7 @@
       <c r="E28" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F28" s="83"/>
+      <c r="F28" s="92"/>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D29" s="3" t="s">
@@ -2185,7 +2186,7 @@
       <c r="E29" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="84"/>
+      <c r="F29" s="93"/>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
@@ -2194,7 +2195,7 @@
       <c r="E30" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F30" s="84"/>
+      <c r="F30" s="93"/>
     </row>
     <row r="31" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D31" s="3" t="s">
@@ -2203,7 +2204,7 @@
       <c r="E31" s="13">
         <v>5</v>
       </c>
-      <c r="F31" s="84"/>
+      <c r="F31" s="93"/>
     </row>
     <row r="32" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D32" s="4" t="s">
@@ -2212,14 +2213,14 @@
       <c r="E32" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="85"/>
+      <c r="F32" s="94"/>
     </row>
     <row r="33" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" s="105" t="s">
+      <c r="D34" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="E34" s="106"/>
+      <c r="E34" s="102"/>
       <c r="F34" s="28" t="s">
         <v>16</v>
       </c>
@@ -2231,7 +2232,7 @@
       <c r="E35" s="22">
         <v>37</v>
       </c>
-      <c r="F35" s="98"/>
+      <c r="F35" s="67"/>
     </row>
     <row r="36" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D36" s="11" t="s">
@@ -2240,7 +2241,7 @@
       <c r="E36" s="22">
         <v>60</v>
       </c>
-      <c r="F36" s="99"/>
+      <c r="F36" s="68"/>
     </row>
     <row r="37" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D37" s="12" t="s">
@@ -2249,7 +2250,7 @@
       <c r="E37" s="23">
         <v>0</v>
       </c>
-      <c r="F37" s="100"/>
+      <c r="F37" s="69"/>
     </row>
     <row r="38" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
@@ -2268,7 +2269,7 @@
       <c r="E40" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="F40" s="83"/>
+      <c r="F40" s="92"/>
     </row>
     <row r="41" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D41" s="3" t="s">
@@ -2277,7 +2278,7 @@
       <c r="E41" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F41" s="84"/>
+      <c r="F41" s="93"/>
     </row>
     <row r="42" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D42" s="3" t="s">
@@ -2286,7 +2287,7 @@
       <c r="E42" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="84"/>
+      <c r="F42" s="93"/>
     </row>
     <row r="43" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D43" s="3" t="s">
@@ -2295,7 +2296,7 @@
       <c r="E43" s="13">
         <v>6</v>
       </c>
-      <c r="F43" s="84"/>
+      <c r="F43" s="93"/>
     </row>
     <row r="44" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D44" s="4" t="s">
@@ -2304,14 +2305,14 @@
       <c r="E44" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F44" s="85"/>
+      <c r="F44" s="94"/>
     </row>
     <row r="45" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D46" s="105" t="s">
+      <c r="D46" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="E46" s="106"/>
+      <c r="E46" s="102"/>
       <c r="F46" s="28" t="s">
         <v>16</v>
       </c>
@@ -2323,7 +2324,7 @@
       <c r="E47" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="F47" s="98"/>
+      <c r="F47" s="67"/>
     </row>
     <row r="48" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D48" s="11" t="s">
@@ -2332,7 +2333,7 @@
       <c r="E48" s="22">
         <v>60</v>
       </c>
-      <c r="F48" s="99"/>
+      <c r="F48" s="68"/>
     </row>
     <row r="49" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="12" t="s">
@@ -2341,14 +2342,14 @@
       <c r="E49" s="23">
         <v>0</v>
       </c>
-      <c r="F49" s="100"/>
+      <c r="F49" s="69"/>
     </row>
     <row r="50" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D51" s="101" t="s">
+      <c r="D51" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="E51" s="102"/>
+      <c r="E51" s="108"/>
       <c r="F51" s="51" t="s">
         <v>16</v>
       </c>
@@ -2360,7 +2361,7 @@
       <c r="E52" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="F52" s="61"/>
+      <c r="F52" s="72"/>
     </row>
     <row r="53" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="1" t="s">
@@ -2369,14 +2370,14 @@
       <c r="E53" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F53" s="62"/>
+      <c r="F53" s="73"/>
     </row>
     <row r="54" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D55" s="107" t="s">
+      <c r="D55" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="E55" s="108"/>
+      <c r="E55" s="111"/>
       <c r="F55" s="49" t="s">
         <v>16</v>
       </c>
@@ -2388,7 +2389,7 @@
       <c r="E56" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="F56" s="89"/>
+      <c r="F56" s="98"/>
     </row>
     <row r="57" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D57" s="5" t="s">
@@ -2397,7 +2398,7 @@
       <c r="E57" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F57" s="90"/>
+      <c r="F57" s="99"/>
     </row>
     <row r="58" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D58" s="6" t="s">
@@ -2406,14 +2407,14 @@
       <c r="E58" s="21">
         <v>300</v>
       </c>
-      <c r="F58" s="91"/>
+      <c r="F58" s="100"/>
     </row>
     <row r="59" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="109" t="s">
+      <c r="D60" s="112" t="s">
         <v>4</v>
       </c>
-      <c r="E60" s="110"/>
+      <c r="E60" s="113"/>
       <c r="F60" s="25" t="s">
         <v>16</v>
       </c>
@@ -2426,7 +2427,7 @@
         <f>Worklist!F1</f>
         <v>Digestion Pathway</v>
       </c>
-      <c r="F61" s="77"/>
+      <c r="F61" s="86"/>
     </row>
     <row r="62" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D62" s="9" t="s">
@@ -2435,7 +2436,7 @@
       <c r="E62" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F62" s="78"/>
+      <c r="F62" s="87"/>
     </row>
     <row r="63" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D63" s="10" t="s">
@@ -2444,21 +2445,21 @@
       <c r="E63" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F63" s="79"/>
+      <c r="F63" s="88"/>
     </row>
     <row r="64" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B65" s="69" t="s">
+      <c r="B65" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="70"/>
+      <c r="C65" s="71"/>
       <c r="D65" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="F65" s="101" t="s">
+      <c r="F65" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="G65" s="102"/>
+      <c r="G65" s="108"/>
       <c r="H65" s="51" t="s">
         <v>16</v>
       </c>
@@ -2470,14 +2471,14 @@
       <c r="C66" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D66" s="61"/>
+      <c r="D66" s="72"/>
       <c r="F66" s="31" t="s">
         <v>1</v>
       </c>
       <c r="G66" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="H66" s="61"/>
+      <c r="H66" s="72"/>
     </row>
     <row r="67" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="1" t="s">
@@ -2486,14 +2487,14 @@
       <c r="C67" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="D67" s="62"/>
+      <c r="D67" s="73"/>
       <c r="F67" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G67" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="H67" s="62"/>
+      <c r="H67" s="73"/>
     </row>
     <row r="68" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="24"/>
@@ -2504,10 +2505,10 @@
       <c r="H68" s="57"/>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="94" t="s">
+      <c r="B69" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C69" s="95"/>
+      <c r="C69" s="64"/>
       <c r="D69" s="50" t="s">
         <v>16</v>
       </c>
@@ -2526,14 +2527,14 @@
       <c r="C70" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="D70" s="83"/>
+      <c r="D70" s="92"/>
       <c r="F70" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G70" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H70" s="83"/>
+      <c r="H70" s="92"/>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
@@ -2542,14 +2543,14 @@
       <c r="C71" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D71" s="84"/>
+      <c r="D71" s="93"/>
       <c r="F71" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G71" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="H71" s="84"/>
+      <c r="H71" s="93"/>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
@@ -2558,14 +2559,14 @@
       <c r="C72" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="84"/>
+      <c r="D72" s="93"/>
       <c r="F72" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G72" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H72" s="84"/>
+      <c r="H72" s="93"/>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
@@ -2574,14 +2575,14 @@
       <c r="C73" s="13">
         <v>250</v>
       </c>
-      <c r="D73" s="84"/>
+      <c r="D73" s="93"/>
       <c r="F73" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G73" s="13">
         <v>250</v>
       </c>
-      <c r="H73" s="84"/>
+      <c r="H73" s="93"/>
     </row>
     <row r="74" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B74" s="4" t="s">
@@ -2590,21 +2591,21 @@
       <c r="C74" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="D74" s="85"/>
+      <c r="D74" s="94"/>
       <c r="F74" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G74" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H74" s="85"/>
+      <c r="H74" s="94"/>
     </row>
     <row r="75" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="94" t="s">
+      <c r="B76" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C76" s="95"/>
+      <c r="C76" s="64"/>
       <c r="D76" s="50" t="s">
         <v>16</v>
       </c>
@@ -2623,14 +2624,14 @@
       <c r="C77" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D77" s="83"/>
+      <c r="D77" s="92"/>
       <c r="F77" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G77" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H77" s="83"/>
+      <c r="H77" s="92"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
@@ -2639,14 +2640,14 @@
       <c r="C78" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D78" s="84"/>
+      <c r="D78" s="93"/>
       <c r="F78" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="H78" s="84"/>
+      <c r="H78" s="93"/>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
@@ -2655,14 +2656,14 @@
       <c r="C79" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D79" s="84"/>
+      <c r="D79" s="93"/>
       <c r="F79" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="H79" s="84"/>
+      <c r="H79" s="93"/>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
@@ -2671,14 +2672,14 @@
       <c r="C80" s="13">
         <v>3.6</v>
       </c>
-      <c r="D80" s="84"/>
+      <c r="D80" s="93"/>
       <c r="F80" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G80" s="13">
         <v>30</v>
       </c>
-      <c r="H80" s="84"/>
+      <c r="H80" s="93"/>
     </row>
     <row r="81" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B81" s="4" t="s">
@@ -2687,28 +2688,28 @@
       <c r="C81" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D81" s="85"/>
+      <c r="D81" s="94"/>
       <c r="F81" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G81" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H81" s="85"/>
+      <c r="H81" s="94"/>
     </row>
     <row r="82" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="67" t="s">
+      <c r="B83" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C83" s="68"/>
+      <c r="C83" s="79"/>
       <c r="D83" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F83" s="105" t="s">
+      <c r="F83" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="G83" s="106"/>
+      <c r="G83" s="102"/>
       <c r="H83" s="28" t="s">
         <v>16</v>
       </c>
@@ -2720,14 +2721,14 @@
       <c r="C84" s="22">
         <v>37</v>
       </c>
-      <c r="D84" s="98"/>
+      <c r="D84" s="67"/>
       <c r="F84" s="11" t="s">
         <v>13</v>
       </c>
       <c r="G84" s="22">
         <v>37</v>
       </c>
-      <c r="H84" s="98"/>
+      <c r="H84" s="67"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="11" t="s">
@@ -2737,14 +2738,14 @@
         <f>18*60</f>
         <v>1080</v>
       </c>
-      <c r="D85" s="99"/>
+      <c r="D85" s="68"/>
       <c r="F85" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G85" s="22">
         <v>5000</v>
       </c>
-      <c r="H85" s="99"/>
+      <c r="H85" s="68"/>
     </row>
     <row r="86" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B86" s="12" t="s">
@@ -2753,21 +2754,21 @@
       <c r="C86" s="23">
         <v>0</v>
       </c>
-      <c r="D86" s="100"/>
+      <c r="D86" s="69"/>
       <c r="F86" s="12" t="s">
         <v>21</v>
       </c>
       <c r="G86" s="23">
         <v>0</v>
       </c>
-      <c r="H86" s="100"/>
+      <c r="H86" s="69"/>
     </row>
     <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="94" t="s">
+      <c r="B88" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C88" s="95"/>
+      <c r="C88" s="64"/>
       <c r="D88" s="50" t="s">
         <v>16</v>
       </c>
@@ -2786,14 +2787,14 @@
       <c r="C89" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D89" s="83"/>
+      <c r="D89" s="92"/>
       <c r="F89" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G89" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H89" s="83"/>
+      <c r="H89" s="92"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
@@ -2802,14 +2803,14 @@
       <c r="C90" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D90" s="84"/>
+      <c r="D90" s="93"/>
       <c r="F90" s="3" t="s">
         <v>66</v>
       </c>
       <c r="G90" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H90" s="84"/>
+      <c r="H90" s="93"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
@@ -2818,14 +2819,14 @@
       <c r="C91" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D91" s="84"/>
+      <c r="D91" s="93"/>
       <c r="F91" s="3" t="s">
         <v>64</v>
       </c>
       <c r="G91" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="H91" s="84"/>
+      <c r="H91" s="93"/>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
@@ -2834,14 +2835,14 @@
       <c r="C92" s="55">
         <v>30</v>
       </c>
-      <c r="D92" s="84"/>
+      <c r="D92" s="93"/>
       <c r="F92" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G92" s="13">
         <v>14.2</v>
       </c>
-      <c r="H92" s="84"/>
+      <c r="H92" s="93"/>
     </row>
     <row r="93" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B93" s="4" t="s">
@@ -2850,28 +2851,28 @@
       <c r="C93" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D93" s="85"/>
+      <c r="D93" s="94"/>
       <c r="F93" s="4" t="s">
         <v>45</v>
       </c>
       <c r="G93" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="H93" s="85"/>
+      <c r="H93" s="94"/>
     </row>
     <row r="94" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="67" t="s">
+      <c r="B95" s="78" t="s">
         <v>43</v>
       </c>
-      <c r="C95" s="68"/>
+      <c r="C95" s="79"/>
       <c r="D95" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="F95" s="101" t="s">
+      <c r="F95" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="G95" s="102"/>
+      <c r="G95" s="108"/>
       <c r="H95" s="51" t="s">
         <v>16</v>
       </c>
@@ -2883,10 +2884,10 @@
       <c r="C96" s="22">
         <v>37</v>
       </c>
-      <c r="D96" s="98"/>
-      <c r="F96" s="63"/>
-      <c r="G96" s="64"/>
-      <c r="H96" s="61"/>
+      <c r="D96" s="67"/>
+      <c r="F96" s="74"/>
+      <c r="G96" s="75"/>
+      <c r="H96" s="72"/>
     </row>
     <row r="97" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B97" s="11" t="s">
@@ -2896,10 +2897,10 @@
         <f>60*4</f>
         <v>240</v>
       </c>
-      <c r="D97" s="99"/>
-      <c r="F97" s="65"/>
-      <c r="G97" s="66"/>
-      <c r="H97" s="62"/>
+      <c r="D97" s="68"/>
+      <c r="F97" s="76"/>
+      <c r="G97" s="77"/>
+      <c r="H97" s="73"/>
     </row>
     <row r="98" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B98" s="12" t="s">
@@ -2908,14 +2909,14 @@
       <c r="C98" s="23">
         <v>0</v>
       </c>
-      <c r="D98" s="100"/>
+      <c r="D98" s="69"/>
     </row>
     <row r="99" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="94" t="s">
+      <c r="B100" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C100" s="95"/>
+      <c r="C100" s="64"/>
       <c r="D100" s="50" t="s">
         <v>16</v>
       </c>
@@ -2927,7 +2928,7 @@
       <c r="C101" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D101" s="83"/>
+      <c r="D101" s="92"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
@@ -2936,7 +2937,7 @@
       <c r="C102" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D102" s="84"/>
+      <c r="D102" s="93"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
@@ -2945,7 +2946,7 @@
       <c r="C103" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="D103" s="84"/>
+      <c r="D103" s="93"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
@@ -2954,7 +2955,7 @@
       <c r="C104" s="13">
         <v>14.2</v>
       </c>
-      <c r="D104" s="84"/>
+      <c r="D104" s="93"/>
     </row>
     <row r="105" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B105" s="4" t="s">
@@ -2963,27 +2964,27 @@
       <c r="C105" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D105" s="85"/>
+      <c r="D105" s="94"/>
     </row>
     <row r="106" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="107" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B107" s="101" t="s">
+      <c r="B107" s="107" t="s">
         <v>63</v>
       </c>
-      <c r="C107" s="102"/>
+      <c r="C107" s="108"/>
       <c r="D107" s="58" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B108" s="63"/>
-      <c r="C108" s="64"/>
-      <c r="D108" s="61"/>
+      <c r="B108" s="74"/>
+      <c r="C108" s="75"/>
+      <c r="D108" s="72"/>
     </row>
     <row r="109" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B109" s="65"/>
-      <c r="C109" s="66"/>
-      <c r="D109" s="62"/>
+      <c r="B109" s="76"/>
+      <c r="C109" s="77"/>
+      <c r="D109" s="73"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K111" s="24"/>
@@ -3023,19 +3024,31 @@
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F35:F37"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="H89:H93"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="H84:H86"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D89:D93"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="F95:G95"/>
+    <mergeCell ref="B108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="F96:G97"/>
+    <mergeCell ref="H96:H97"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="D101:D105"/>
+    <mergeCell ref="D96:D98"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="B83:C83"/>
+    <mergeCell ref="D84:D86"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="H77:H81"/>
+    <mergeCell ref="F83:G83"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="F76:G76"/>
+    <mergeCell ref="F69:G69"/>
     <mergeCell ref="H70:H74"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="B65:C65"/>
@@ -3051,31 +3064,19 @@
     <mergeCell ref="F52:F53"/>
     <mergeCell ref="F61:F63"/>
     <mergeCell ref="F40:F44"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="F76:G76"/>
-    <mergeCell ref="F69:G69"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="B83:C83"/>
-    <mergeCell ref="D84:D86"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="H77:H81"/>
-    <mergeCell ref="F83:G83"/>
-    <mergeCell ref="B108:C109"/>
-    <mergeCell ref="D108:D109"/>
-    <mergeCell ref="F96:G97"/>
-    <mergeCell ref="H96:H97"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="D101:D105"/>
-    <mergeCell ref="D96:D98"/>
-    <mergeCell ref="H89:H93"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="H84:H86"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D89:D93"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="F95:G95"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F28:F32"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="D27:E27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3160,7 +3161,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3247,7 +3248,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
         <v>85</v>
@@ -3315,18 +3316,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3553,18 +3554,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158388FD-FCB9-4D40-8807-AFB22AE8C172}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46E792D2-13D9-445F-AE7B-CF179A33399C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46E792D2-13D9-445F-AE7B-CF179A33399C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158388FD-FCB9-4D40-8807-AFB22AE8C172}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Added PreRun and Init to Hamilton Commands.
</commit_message>
<xml_diff>
--- a/Method Maker1.xlsx
+++ b/Method Maker1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonMethodMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0E81B4-CD6B-4B97-9A56-C4A9AA83369C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB47EF4B-78A0-4C86-8EF8-7E0CD4B442CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1065" windowWidth="15300" windowHeight="11055" firstSheet="1" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
+    <workbookView xWindow="1395" yWindow="1065" windowWidth="15300" windowHeight="11055" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="___Dropdown values" sheetId="4" r:id="rId1"/>
@@ -1296,7 +1296,7 @@
   <dimension ref="B3:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B7"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1364,7 @@
         <v>68</v>
       </c>
       <c r="D5" s="49">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -1392,9 +1392,7 @@
       <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="49">
-        <v>200</v>
-      </c>
+      <c r="D6" s="49"/>
       <c r="F6" t="s">
         <v>30</v>
       </c>
@@ -1421,26 +1419,22 @@
       <c r="B7" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="49">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D8" s="49">
-        <v>300</v>
-      </c>
+      <c r="D7" s="49"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="43" t="s">
         <v>66</v>
       </c>
+      <c r="D9" s="35" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="35" t="s">
-        <v>62</v>
+      <c r="D10" s="24" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -1448,15 +1442,12 @@
         <v>74</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>75</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -1840,7 +1831,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0EB2AB26-95FB-457C-BC05-2F40488B0593}">
           <x14:formula1>
-            <xm:f>'___Dropdown values'!$D$11:$D$12</xm:f>
+            <xm:f>'___Dropdown values'!$D$10:$D$11</xm:f>
           </x14:formula1>
           <xm:sqref>H15 L10</xm:sqref>
         </x14:dataValidation>
@@ -1870,7 +1861,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FB148A77-7292-4C2D-A64A-C8315CF04711}">
           <x14:formula1>
-            <xm:f>'___Dropdown values'!$D$4:$D$8</xm:f>
+            <xm:f>'___Dropdown values'!$D$4:$D$7</xm:f>
           </x14:formula1>
           <xm:sqref>L6</xm:sqref>
         </x14:dataValidation>
@@ -1886,7 +1877,7 @@
   <dimension ref="B1:O121"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,9 +3114,9 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1EA7122-9BB0-47F3-A320-6D1AE93FB4E0}">
           <x14:formula1>
-            <xm:f>'___Dropdown values'!$D$11:$D$12</xm:f>
+            <xm:f>'___Dropdown values'!$D$10:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E17 E32 E49 C86 G86 C98 C110 G98 C79 G79 E40</xm:sqref>
+          <xm:sqref>E17 E40 G79 C79 G98 C110 C98 G86 C86 E49 E32</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6BE6F825-91BE-4CEC-9D14-5710077D0618}">
           <x14:formula1>
@@ -3138,12 +3129,6 @@
             <xm:f>'___Dropdown values'!$K$5:$K$6</xm:f>
           </x14:formula1>
           <xm:sqref>D34:E34 D51:E51 B88:C88 F88:G88 B100:C100</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C124AD9A-B163-4E82-86EB-DE4F7DADE970}">
-          <x14:formula1>
-            <xm:f>'___Dropdown values'!$D$4:$D$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>E63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{345D99D0-6529-4A67-8275-A029C65E5115}">
           <x14:formula1>
@@ -3162,6 +3147,12 @@
             <xm:f>'___Dropdown values'!$I$5:$I$6</xm:f>
           </x14:formula1>
           <xm:sqref>D39:E39</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C124AD9A-B163-4E82-86EB-DE4F7DADE970}">
+          <x14:formula1>
+            <xm:f>'___Dropdown values'!$D$4:$D$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E63</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Adding a way to do pre-init for Hamilton libraries if needed.
</commit_message>
<xml_diff>
--- a/Method Maker1.xlsx
+++ b/Method Maker1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonMethodMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB47EF4B-78A0-4C86-8EF8-7E0CD4B442CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21951AE4-0D10-4E97-8FD8-C537AD52A782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1065" windowWidth="15300" windowHeight="11055" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
+    <workbookView xWindow="1395" yWindow="1065" windowWidth="15300" windowHeight="11055" activeTab="1" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="___Dropdown values" sheetId="4" r:id="rId1"/>
@@ -1504,8 +1504,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C2:Q20"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1876,7 +1876,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="C37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added PreRun information. Moved step preferred loading to SystemConfiguration.yaml.
</commit_message>
<xml_diff>
--- a/Method Maker1.xlsx
+++ b/Method Maker1.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonMethodMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21951AE4-0D10-4E97-8FD8-C537AD52A782}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D105B5CC-E113-4710-9550-DCB5DE99E82A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1065" windowWidth="15300" windowHeight="11055" activeTab="1" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
+    <workbookView xWindow="6075" yWindow="1650" windowWidth="15300" windowHeight="11055" firstSheet="1" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="___Dropdown values" sheetId="4" r:id="rId1"/>
     <sheet name="Building Blocks" sheetId="1" r:id="rId2"/>
     <sheet name="Method" sheetId="2" r:id="rId3"/>
-    <sheet name="SolutionPrep" sheetId="5" r:id="rId4"/>
-    <sheet name="Worklist" sheetId="3" r:id="rId5"/>
+    <sheet name="Worklist" sheetId="3" r:id="rId4"/>
+    <sheet name="SolutionPrep" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="90">
   <si>
     <t>Liquid Transfer</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>This is a Test Message.\nThank you for reading!</t>
+  </si>
+  <si>
+    <t>Volumes</t>
   </si>
 </sst>
 </file>
@@ -1504,7 +1507,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="C2:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -1876,8 +1879,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:O121"/>
   <sheetViews>
-    <sheetView topLeftCell="C37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2019,8 +2022,8 @@
       <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="13">
-        <v>60</v>
+      <c r="E16" t="s">
+        <v>89</v>
       </c>
       <c r="F16" s="81"/>
       <c r="K16" s="24"/>
@@ -3161,24 +3164,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F70090-C34D-4006-BF44-FF3E7D4D54FA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD529AF6-49B7-49B9-A330-C878FB7908FD}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3199,7 +3190,7 @@
     <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3221,8 +3212,11 @@
       <c r="G1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>ROW(A1)</f>
         <v>1</v>
@@ -3245,8 +3239,11 @@
       <c r="G2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>ROW(A2)</f>
         <v>2</v>
@@ -3270,8 +3267,11 @@
       <c r="G3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>ROW(A3)</f>
         <v>3</v>
@@ -3294,6 +3294,9 @@
       </c>
       <c r="G4" t="s">
         <v>86</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3329,6 +3332,18 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F70090-C34D-4006-BF44-FF3E7D4D54FA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated scripts to support the vacuum step.
</commit_message>
<xml_diff>
--- a/Method Maker1.xlsx
+++ b/Method Maker1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonMethodMaker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\program files (x86)\hamilton\bareb\script\hamiltonmethodmaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C1DD57-4F02-4BAE-B7C1-77CE5E43C548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4901BC-71FF-469B-8169-3CF9065C6773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6975" yWindow="1635" windowWidth="15300" windowHeight="11055" firstSheet="1" activeTab="3" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="___Dropdown values" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="92">
   <si>
     <t>Liquid Transfer</t>
   </si>
@@ -176,9 +176,6 @@
     <t>Mix?</t>
   </si>
   <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Vacuum</t>
   </si>
   <si>
-    <t>Pressure Difference</t>
-  </si>
-  <si>
     <t>Denaturation</t>
   </si>
   <si>
@@ -309,6 +303,15 @@
   </si>
   <si>
     <t>SizeX:100,SizeX:100</t>
+  </si>
+  <si>
+    <t>Pressure Difference (mTorr)</t>
+  </si>
+  <si>
+    <t>Time (sec)</t>
+  </si>
+  <si>
+    <t>Source Plate</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -638,11 +641,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -755,10 +782,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -779,13 +802,106 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -809,98 +925,26 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -908,10 +952,16 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -920,25 +970,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2632,7 +2664,7 @@
       </c>
       <c r="C3" s="43"/>
       <c r="D3" s="43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" s="60" t="s">
         <v>29</v>
@@ -2649,7 +2681,7 @@
         <v>37</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>0</v>
@@ -2664,21 +2696,21 @@
         <v>22</v>
       </c>
       <c r="J4" s="43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K4" s="43" t="s">
         <v>43</v>
       </c>
       <c r="L4" s="43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -2693,13 +2725,13 @@
         <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K5" t="s">
         <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -2720,63 +2752,63 @@
         <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K6" t="s">
         <v>44</v>
       </c>
       <c r="L6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D7" s="49"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -2791,17 +2823,17 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2816,10 +2848,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5792BA43-E664-4C0E-82EF-315A761798FC}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="C2:Q20"/>
+  <dimension ref="C2:Q21"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2846,31 +2878,31 @@
   <sheetData>
     <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="71"/>
-      <c r="E3" s="55" t="s">
+      <c r="D3" s="70"/>
+      <c r="E3" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="80" t="s">
+      <c r="G3" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="81"/>
+      <c r="H3" s="72"/>
       <c r="I3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="84" t="s">
+      <c r="K3" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="85"/>
+      <c r="L3" s="76"/>
       <c r="M3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="78" t="s">
+      <c r="O3" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="79"/>
+      <c r="P3" s="68"/>
       <c r="Q3" s="28" t="s">
         <v>16</v>
       </c>
@@ -2880,74 +2912,74 @@
         <v>1</v>
       </c>
       <c r="D4" s="34"/>
-      <c r="E4" s="72"/>
+      <c r="E4" s="61"/>
       <c r="G4" s="7" t="s">
         <v>42</v>
       </c>
       <c r="H4" s="15"/>
-      <c r="I4" s="95"/>
+      <c r="I4" s="86"/>
       <c r="K4" s="5" t="s">
         <v>42</v>
       </c>
       <c r="L4" s="20"/>
-      <c r="M4" s="98"/>
+      <c r="M4" s="89"/>
       <c r="O4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="P4" s="22"/>
-      <c r="Q4" s="67"/>
+      <c r="Q4" s="96"/>
     </row>
     <row r="5" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="56" t="s">
+      <c r="C5" s="54" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="33"/>
-      <c r="E5" s="73"/>
+      <c r="E5" s="62"/>
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="96"/>
+      <c r="I5" s="87"/>
       <c r="K5" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L5" s="20"/>
-      <c r="M5" s="99"/>
+      <c r="M5" s="90"/>
       <c r="O5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="P5" s="22"/>
-      <c r="Q5" s="68"/>
+      <c r="Q5" s="97"/>
     </row>
     <row r="6" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="15"/>
-      <c r="I6" s="96"/>
+      <c r="I6" s="87"/>
       <c r="K6" s="6" t="s">
         <v>41</v>
       </c>
       <c r="L6" s="21"/>
-      <c r="M6" s="100"/>
+      <c r="M6" s="91"/>
       <c r="O6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="P6" s="23"/>
-      <c r="Q6" s="69"/>
+      <c r="Q6" s="98"/>
     </row>
     <row r="7" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="15"/>
-      <c r="I7" s="96"/>
+      <c r="I7" s="87"/>
     </row>
     <row r="8" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="83"/>
+      <c r="D8" s="74"/>
       <c r="E8" s="25" t="s">
         <v>16</v>
       </c>
@@ -2955,144 +2987,143 @@
         <v>11</v>
       </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="97"/>
+      <c r="I8" s="88"/>
     </row>
     <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="86"/>
-      <c r="K9" s="70" t="s">
+      <c r="E9" s="77"/>
+      <c r="K9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="71"/>
+      <c r="L9" s="70"/>
       <c r="M9" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="O9" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="P9" s="79"/>
-      <c r="Q9" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="18"/>
-      <c r="E10" s="87"/>
-      <c r="G10" s="63" t="s">
+      <c r="E10" s="78"/>
+      <c r="G10" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="64"/>
+      <c r="H10" s="93"/>
       <c r="I10" s="29" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L10" s="32"/>
-      <c r="M10" s="89"/>
-      <c r="O10" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="P10" s="50"/>
-      <c r="Q10" s="51"/>
+      <c r="M10" s="80"/>
     </row>
     <row r="11" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="88"/>
+      <c r="E11" s="79"/>
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="13"/>
-      <c r="I11" s="92"/>
+      <c r="I11" s="83"/>
       <c r="K11" s="31" t="s">
         <v>23</v>
       </c>
       <c r="L11" s="32"/>
-      <c r="M11" s="90"/>
+      <c r="M11" s="81"/>
     </row>
     <row r="12" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H12" s="13"/>
-      <c r="I12" s="93"/>
+      <c r="I12" s="84"/>
       <c r="K12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="L12" s="33"/>
-      <c r="M12" s="91"/>
+      <c r="M12" s="82"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C13" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="D13" s="71"/>
+      <c r="C13" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="70"/>
       <c r="E13" s="44" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H13" s="13"/>
-      <c r="I13" s="93"/>
+      <c r="I13" s="84"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="74"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="72"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="61"/>
       <c r="G14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="13"/>
-      <c r="I14" s="93"/>
+      <c r="I14" s="84"/>
     </row>
     <row r="15" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="76"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="73"/>
+      <c r="C15" s="65"/>
+      <c r="D15" s="66"/>
+      <c r="E15" s="62"/>
       <c r="G15" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="I15" s="94"/>
+        <v>46</v>
+      </c>
+      <c r="I15" s="85"/>
     </row>
     <row r="17" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G18" s="65" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="66"/>
+      <c r="G18" s="94" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="95"/>
       <c r="I18" s="36" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="38"/>
-      <c r="I19" s="61"/>
-    </row>
-    <row r="20" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G20" s="39" t="s">
-        <v>46</v>
-      </c>
-      <c r="H20" s="40"/>
-      <c r="I20" s="62"/>
+      <c r="G19" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="H19" s="59"/>
+      <c r="I19" s="99"/>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="H20" s="38"/>
+      <c r="I20" s="100"/>
+    </row>
+    <row r="21" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G21" s="39" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21" s="40"/>
+      <c r="I21" s="101"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="19">
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I19:I21"/>
     <mergeCell ref="E4:E5"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="C14:D15"/>
@@ -3104,21 +3135,16 @@
     <mergeCell ref="E9:E11"/>
     <mergeCell ref="M10:M12"/>
     <mergeCell ref="I11:I15"/>
-    <mergeCell ref="O9:P9"/>
     <mergeCell ref="I4:I8"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="I19:I20"/>
     <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="K9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{87B7FEB9-4E8E-42EA-B6C5-6BC938B15EDF}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$B$20:$B$21</xm:f>
@@ -3148,12 +3174,6 @@
             <xm:f>'___Dropdown values'!$D$10:$D$11</xm:f>
           </x14:formula1>
           <xm:sqref>H15 L10</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D24472BE-C623-4AB4-94FD-D9A2A0078F32}">
-          <x14:formula1>
-            <xm:f>'___Dropdown values'!$L$5:$L$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>O9:P9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DCE90996-E256-430A-ADF7-A9ADA249193A}">
           <x14:formula1>
@@ -3188,10 +3208,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88364F8-85B5-4C5D-8958-0F9155266F29}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B1:O122"/>
+  <dimension ref="B1:O121"/>
   <sheetViews>
-    <sheetView topLeftCell="D6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C26" sqref="A26:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3212,10 +3232,10 @@
   <sheetData>
     <row r="1" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="70" t="s">
+      <c r="D2" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="71"/>
+      <c r="E2" s="70"/>
       <c r="F2" s="30" t="s">
         <v>16</v>
       </c>
@@ -3227,8 +3247,8 @@
       <c r="E3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="72" t="s">
-        <v>56</v>
+      <c r="F3" s="61" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3238,20 +3258,20 @@
       <c r="E4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="73"/>
+      <c r="F4" s="62"/>
     </row>
     <row r="6" spans="4:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="109" t="s">
+      <c r="D6" s="114" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="109"/>
+      <c r="E6" s="114"/>
     </row>
     <row r="7" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="107" t="s">
+      <c r="D8" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="108"/>
+      <c r="E8" s="105"/>
       <c r="F8" s="41" t="s">
         <v>16</v>
       </c>
@@ -3261,9 +3281,9 @@
         <v>1</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="105"/>
+        <v>49</v>
+      </c>
+      <c r="F9" s="112"/>
     </row>
     <row r="10" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
@@ -3272,7 +3292,7 @@
       <c r="E10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="106"/>
+      <c r="F10" s="113"/>
     </row>
     <row r="11" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I11" s="24"/>
@@ -3281,10 +3301,10 @@
       <c r="O11"/>
     </row>
     <row r="12" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D12" s="103" t="s">
+      <c r="D12" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="104"/>
+      <c r="E12" s="103"/>
       <c r="F12" s="47" t="s">
         <v>16</v>
       </c>
@@ -3299,18 +3319,18 @@
         <f>Worklist!G1</f>
         <v>1st Pipetting Step</v>
       </c>
-      <c r="F13" s="92"/>
+      <c r="F13" s="83"/>
       <c r="N13"/>
       <c r="O13"/>
     </row>
     <row r="14" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="93"/>
+        <v>75</v>
+      </c>
+      <c r="F14" s="84"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="N14"/>
@@ -3318,12 +3338,12 @@
     </row>
     <row r="15" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="93"/>
+        <v>68</v>
+      </c>
+      <c r="F15" s="84"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="N15"/>
@@ -3336,7 +3356,7 @@
       <c r="E16">
         <v>10</v>
       </c>
-      <c r="F16" s="93"/>
+      <c r="F16" s="84"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="N16"/>
@@ -3347,9 +3367,9 @@
         <v>45</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="94"/>
+        <v>46</v>
+      </c>
+      <c r="F17" s="85"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="N17"/>
@@ -3362,10 +3382,10 @@
       <c r="O18"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="81"/>
+      <c r="E19" s="72"/>
       <c r="F19" s="26" t="s">
         <v>16</v>
       </c>
@@ -3381,7 +3401,7 @@
       <c r="E20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="95"/>
+      <c r="F20" s="86"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="N20"/>
@@ -3394,7 +3414,7 @@
       <c r="E21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="96"/>
+      <c r="F21" s="87"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="N21"/>
@@ -3408,7 +3428,7 @@
         <f>Worklist!E1</f>
         <v>_Conc</v>
       </c>
-      <c r="F22" s="96"/>
+      <c r="F22" s="87"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="N22"/>
@@ -3421,7 +3441,7 @@
       <c r="E23" s="15">
         <v>10</v>
       </c>
-      <c r="F23" s="96"/>
+      <c r="F23" s="87"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="N23"/>
@@ -3434,885 +3454,890 @@
       <c r="E24" s="16">
         <v>50</v>
       </c>
-      <c r="F24" s="97"/>
+      <c r="F24" s="88"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="N24"/>
       <c r="O24"/>
     </row>
-    <row r="25" spans="4:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K25" s="24"/>
       <c r="L25" s="24"/>
       <c r="N25"/>
       <c r="O25"/>
     </row>
-    <row r="26" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="4:15" x14ac:dyDescent="0.25">
+      <c r="D26" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" s="103"/>
+      <c r="F26" s="47" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="27" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D27" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="104"/>
-      <c r="F27" s="47" t="s">
-        <v>16</v>
-      </c>
+      <c r="D27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F27" s="83"/>
     </row>
     <row r="28" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D28" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" s="92"/>
+        <v>63</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F28" s="84"/>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D29" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="F29" s="93"/>
+        <v>68</v>
+      </c>
+      <c r="F29" s="84"/>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" s="93"/>
-    </row>
-    <row r="31" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D31" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E31" s="13">
+      <c r="E30" s="13">
         <v>5</v>
       </c>
-      <c r="F31" s="93"/>
-    </row>
-    <row r="32" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="4" t="s">
+      <c r="F30" s="84"/>
+    </row>
+    <row r="31" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F32" s="94"/>
-    </row>
-    <row r="33" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="E31" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="85"/>
+    </row>
+    <row r="32" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D33" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="107"/>
+      <c r="F33" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" s="101" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="102"/>
-      <c r="F34" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="D34" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="22">
+        <v>37</v>
+      </c>
+      <c r="F34" s="96"/>
     </row>
     <row r="35" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D35" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E35" s="22">
-        <v>37</v>
-      </c>
-      <c r="F35" s="67"/>
-    </row>
-    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D36" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="22">
         <v>60</v>
       </c>
-      <c r="F36" s="68"/>
-    </row>
-    <row r="37" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="12" t="s">
+      <c r="F35" s="97"/>
+    </row>
+    <row r="36" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="23">
+      <c r="E36" s="23">
         <v>0</v>
       </c>
-      <c r="F37" s="69"/>
-    </row>
-    <row r="38" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="F36" s="98"/>
+    </row>
+    <row r="37" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D38" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="70"/>
+      <c r="F38" s="45" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="39" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D39" s="70" t="s">
-        <v>22</v>
-      </c>
-      <c r="E39" s="71"/>
-      <c r="F39" s="45" t="s">
-        <v>16</v>
-      </c>
+      <c r="D39" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="80"/>
     </row>
     <row r="40" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D40" s="31" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="E40" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="F40" s="89"/>
-    </row>
-    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D41" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="F41" s="90"/>
-    </row>
-    <row r="42" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" s="81"/>
+    </row>
+    <row r="41" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E42" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="F42" s="91"/>
-    </row>
-    <row r="43" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="E41" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="F41" s="82"/>
+    </row>
+    <row r="42" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D43" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="103"/>
+      <c r="F43" s="47" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="44" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D44" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="E44" s="104"/>
-      <c r="F44" s="47" t="s">
-        <v>16</v>
-      </c>
+      <c r="D44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F44" s="83"/>
     </row>
     <row r="45" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D45" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F45" s="92"/>
+        <v>72</v>
+      </c>
+      <c r="F45" s="84"/>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D46" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F46" s="93"/>
+        <v>68</v>
+      </c>
+      <c r="F46" s="84"/>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D47" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F47" s="93"/>
-    </row>
-    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D48" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E47" s="13">
         <v>301</v>
       </c>
-      <c r="F48" s="93"/>
-    </row>
-    <row r="49" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D49" s="4" t="s">
+      <c r="F47" s="84"/>
+    </row>
+    <row r="48" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D48" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E49" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="F49" s="94"/>
-    </row>
-    <row r="50" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="E48" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F48" s="85"/>
+    </row>
+    <row r="49" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D50" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" s="107"/>
+      <c r="F50" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="51" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D51" s="101" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="102"/>
-      <c r="F51" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="D51" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="F51" s="96"/>
     </row>
     <row r="52" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D52" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="F52" s="67"/>
-    </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D53" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="22">
+      <c r="E52" s="22">
         <v>60</v>
       </c>
-      <c r="F53" s="68"/>
-    </row>
-    <row r="54" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D54" s="12" t="s">
+      <c r="F52" s="97"/>
+    </row>
+    <row r="53" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D53" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E54" s="23">
+      <c r="E53" s="23">
         <v>0</v>
       </c>
-      <c r="F54" s="69"/>
-    </row>
-    <row r="55" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="F53" s="98"/>
+    </row>
+    <row r="54" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D55" s="104" t="s">
+        <v>2</v>
+      </c>
+      <c r="E55" s="105"/>
+      <c r="F55" s="48" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="56" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="107" t="s">
-        <v>2</v>
-      </c>
-      <c r="E56" s="108"/>
-      <c r="F56" s="48" t="s">
+      <c r="D56" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="34" t="s">
+        <v>77</v>
+      </c>
+      <c r="F56" s="61"/>
+    </row>
+    <row r="57" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="F57" s="62"/>
+    </row>
+    <row r="58" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D59" s="108" t="s">
+        <v>5</v>
+      </c>
+      <c r="E59" s="109"/>
+      <c r="F59" s="46" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D57" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E57" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="F57" s="72"/>
-    </row>
-    <row r="58" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D58" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E58" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="F58" s="73"/>
-    </row>
-    <row r="59" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="60" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="110" t="s">
-        <v>5</v>
-      </c>
-      <c r="E60" s="111"/>
-      <c r="F60" s="46" t="s">
-        <v>16</v>
-      </c>
+      <c r="D60" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F60" s="89"/>
     </row>
     <row r="61" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D61" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E61" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="F61" s="98"/>
-    </row>
-    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D62" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E62" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F62" s="99"/>
-    </row>
-    <row r="63" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D63" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F61" s="90"/>
+    </row>
+    <row r="62" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D62" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="F63" s="100"/>
-    </row>
-    <row r="64" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D64" s="57"/>
-      <c r="E64" s="58"/>
-      <c r="F64" s="59"/>
-    </row>
-    <row r="65" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="E62" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F62" s="91"/>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="55"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="57"/>
+    </row>
+    <row r="64" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D65" s="110" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="111"/>
+      <c r="F65" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D66" s="112" t="s">
-        <v>4</v>
-      </c>
-      <c r="E66" s="113"/>
-      <c r="F66" s="25" t="s">
-        <v>16</v>
-      </c>
+      <c r="D66" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="18" t="str">
+        <f>Worklist!F1</f>
+        <v>Digestion Pathway</v>
+      </c>
+      <c r="F66" s="77"/>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D67" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E67" s="18" t="str">
-        <f>Worklist!F1</f>
-        <v>Digestion Pathway</v>
-      </c>
-      <c r="F67" s="86"/>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D68" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E68" s="18" t="s">
+      <c r="E67" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F68" s="87"/>
-    </row>
-    <row r="69" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D69" s="10" t="s">
+      <c r="F67" s="78"/>
+    </row>
+    <row r="68" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D68" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E69" s="19" t="s">
+      <c r="E68" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="F69" s="88"/>
-    </row>
-    <row r="70" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="F68" s="79"/>
+    </row>
+    <row r="69" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="70"/>
+      <c r="D70" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="F70" s="104" t="s">
+        <v>2</v>
+      </c>
+      <c r="G70" s="105"/>
+      <c r="H70" s="48" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="C71" s="71"/>
-      <c r="D71" s="48" t="s">
+      <c r="B71" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C71" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" s="61"/>
+      <c r="F71" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G71" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" s="61"/>
+    </row>
+    <row r="72" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C72" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="D72" s="62"/>
+      <c r="F72" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="H72" s="62"/>
+    </row>
+    <row r="73" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B73" s="24"/>
+      <c r="C73" s="51"/>
+      <c r="D73" s="52"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="51"/>
+      <c r="H73" s="52"/>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="C74" s="93"/>
+      <c r="D74" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F71" s="107" t="s">
-        <v>2</v>
-      </c>
-      <c r="G71" s="108"/>
-      <c r="H71" s="48" t="s">
+      <c r="F74" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" s="103"/>
+      <c r="H74" s="47" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="31" t="s">
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C72" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D72" s="72"/>
-      <c r="F72" s="31" t="s">
+      <c r="C75" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D75" s="83"/>
+      <c r="F75" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G72" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="H72" s="72"/>
-    </row>
-    <row r="73" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C73" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D73" s="73"/>
-      <c r="F73" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G73" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="H73" s="73"/>
-    </row>
-    <row r="74" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B74" s="24"/>
-      <c r="C74" s="53"/>
-      <c r="D74" s="54"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="53"/>
-      <c r="H74" s="54"/>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C75" s="64"/>
-      <c r="D75" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="F75" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="G75" s="104"/>
-      <c r="H75" s="47" t="s">
-        <v>16</v>
-      </c>
+      <c r="G75" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H75" s="83"/>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C76" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D76" s="92"/>
+        <v>2</v>
+      </c>
+      <c r="D76" s="84"/>
       <c r="F76" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H76" s="92"/>
+        <v>2</v>
+      </c>
+      <c r="H76" s="84"/>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C77" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D77" s="93"/>
+        <v>68</v>
+      </c>
+      <c r="D77" s="84"/>
       <c r="F77" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H77" s="93"/>
+        <v>68</v>
+      </c>
+      <c r="H77" s="84"/>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C78" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D78" s="93"/>
+        <v>12</v>
+      </c>
+      <c r="C78" s="13">
+        <v>250</v>
+      </c>
+      <c r="D78" s="84"/>
       <c r="F78" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G78" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H78" s="93"/>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C79" s="13">
+      <c r="G78" s="13">
         <v>250</v>
       </c>
-      <c r="D79" s="93"/>
-      <c r="F79" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G79" s="13">
-        <v>250</v>
-      </c>
-      <c r="H79" s="93"/>
-    </row>
-    <row r="80" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="4" t="s">
+      <c r="H78" s="84"/>
+    </row>
+    <row r="79" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C80" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D80" s="94"/>
-      <c r="F80" s="4" t="s">
+      <c r="C79" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D79" s="85"/>
+      <c r="F79" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G80" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="H80" s="94"/>
-    </row>
-    <row r="81" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="G79" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H79" s="85"/>
+    </row>
+    <row r="80" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="93"/>
+      <c r="D81" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F81" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="G81" s="103"/>
+      <c r="H81" s="47" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C82" s="64"/>
-      <c r="D82" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="F82" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="G82" s="104"/>
-      <c r="H82" s="47" t="s">
-        <v>16</v>
-      </c>
+      <c r="B82" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D82" s="83"/>
+      <c r="F82" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G82" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H82" s="83"/>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C83" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="D83" s="92"/>
+        <v>15</v>
+      </c>
+      <c r="D83" s="84"/>
       <c r="F83" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="G83" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="H83" s="92"/>
+        <v>15</v>
+      </c>
+      <c r="H83" s="84"/>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C84" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D84" s="93"/>
+        <v>69</v>
+      </c>
+      <c r="D84" s="84"/>
       <c r="F84" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H84" s="93"/>
+        <v>69</v>
+      </c>
+      <c r="H84" s="84"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C85" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D85" s="93"/>
+        <v>12</v>
+      </c>
+      <c r="C85" s="13">
+        <v>3.6</v>
+      </c>
+      <c r="D85" s="84"/>
       <c r="F85" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G85" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="H85" s="93"/>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C86" s="13">
-        <v>3.6</v>
-      </c>
-      <c r="D86" s="93"/>
-      <c r="F86" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G86" s="13">
+      <c r="G85" s="13">
         <v>30</v>
       </c>
-      <c r="H86" s="93"/>
-    </row>
-    <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B87" s="4" t="s">
+      <c r="H85" s="84"/>
+    </row>
+    <row r="86" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B86" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C87" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D87" s="94"/>
-      <c r="F87" s="4" t="s">
+      <c r="C86" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D86" s="85"/>
+      <c r="F86" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G87" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H87" s="94"/>
-    </row>
-    <row r="88" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="G86" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H86" s="85"/>
+    </row>
+    <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B88" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" s="68"/>
+      <c r="D88" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F88" s="106" t="s">
+        <v>43</v>
+      </c>
+      <c r="G88" s="107"/>
+      <c r="H88" s="28" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="C89" s="79"/>
-      <c r="D89" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F89" s="101" t="s">
-        <v>43</v>
-      </c>
-      <c r="G89" s="102"/>
-      <c r="H89" s="28" t="s">
-        <v>16</v>
-      </c>
+      <c r="B89" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C89" s="22">
+        <v>37</v>
+      </c>
+      <c r="D89" s="96"/>
+      <c r="F89" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G89" s="22">
+        <v>37</v>
+      </c>
+      <c r="H89" s="96"/>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C90" s="22">
-        <v>37</v>
-      </c>
-      <c r="D90" s="67"/>
-      <c r="F90" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G90" s="22">
-        <v>37</v>
-      </c>
-      <c r="H90" s="67"/>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C91" s="22">
         <f>18*60</f>
         <v>1080</v>
       </c>
-      <c r="D91" s="68"/>
-      <c r="F91" s="11" t="s">
+      <c r="D90" s="97"/>
+      <c r="F90" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G91" s="22">
+      <c r="G90" s="22">
         <v>5000</v>
       </c>
-      <c r="H91" s="68"/>
-    </row>
-    <row r="92" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B92" s="12" t="s">
+      <c r="H90" s="97"/>
+    </row>
+    <row r="91" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B91" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C92" s="23">
+      <c r="C91" s="23">
         <v>0</v>
       </c>
-      <c r="D92" s="69"/>
-      <c r="F92" s="12" t="s">
+      <c r="D91" s="98"/>
+      <c r="F91" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="G92" s="23">
+      <c r="G91" s="23">
         <v>0</v>
       </c>
-      <c r="H92" s="69"/>
-    </row>
-    <row r="93" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="H91" s="98"/>
+    </row>
+    <row r="92" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B93" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="C93" s="93"/>
+      <c r="D93" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="F93" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="G93" s="103"/>
+      <c r="H93" s="47" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C94" s="64"/>
-      <c r="D94" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="F94" s="103" t="s">
-        <v>0</v>
-      </c>
-      <c r="G94" s="104"/>
-      <c r="H94" s="47" t="s">
-        <v>16</v>
-      </c>
+      <c r="B94" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C94" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D94" s="83"/>
+      <c r="F94" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G94" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="H94" s="83"/>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C95" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D95" s="92"/>
+        <v>15</v>
+      </c>
+      <c r="D95" s="84"/>
       <c r="F95" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="G95" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="H95" s="92"/>
+        <v>73</v>
+      </c>
+      <c r="H95" s="84"/>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C96" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D96" s="93"/>
+        <v>69</v>
+      </c>
+      <c r="D96" s="84"/>
       <c r="F96" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G96" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="H96" s="93"/>
+        <v>68</v>
+      </c>
+      <c r="H96" s="84"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C97" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="D97" s="93"/>
+        <v>12</v>
+      </c>
+      <c r="C97" s="50">
+        <v>30</v>
+      </c>
+      <c r="D97" s="84"/>
       <c r="F97" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G97" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H97" s="93"/>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C98" s="52">
-        <v>30</v>
-      </c>
-      <c r="D98" s="93"/>
-      <c r="F98" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G98" s="13">
+      <c r="G97" s="13">
         <v>14.2</v>
       </c>
-      <c r="H98" s="93"/>
-    </row>
-    <row r="99" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="4" t="s">
+      <c r="H97" s="84"/>
+    </row>
+    <row r="98" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B98" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C99" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D99" s="94"/>
-      <c r="F99" s="4" t="s">
+      <c r="C98" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D98" s="85"/>
+      <c r="F98" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G99" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H99" s="94"/>
-    </row>
-    <row r="100" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="G98" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="H98" s="85"/>
+    </row>
+    <row r="99" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B100" s="67" t="s">
+        <v>43</v>
+      </c>
+      <c r="C100" s="68"/>
+      <c r="D100" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="F100" s="104" t="s">
+        <v>60</v>
+      </c>
+      <c r="G100" s="105"/>
+      <c r="H100" s="48" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="78" t="s">
-        <v>43</v>
-      </c>
-      <c r="C101" s="79"/>
-      <c r="D101" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F101" s="107" t="s">
-        <v>62</v>
-      </c>
-      <c r="G101" s="108"/>
-      <c r="H101" s="48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B101" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C101" s="22">
+        <v>37</v>
+      </c>
+      <c r="D101" s="96"/>
+      <c r="F101" s="63"/>
+      <c r="G101" s="64"/>
+      <c r="H101" s="61"/>
+    </row>
+    <row r="102" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B102" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C102" s="22">
-        <v>37</v>
-      </c>
-      <c r="D102" s="67"/>
-      <c r="F102" s="74"/>
-      <c r="G102" s="75"/>
-      <c r="H102" s="72"/>
-    </row>
-    <row r="103" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C103" s="22">
         <f>60*4</f>
         <v>240</v>
       </c>
-      <c r="D103" s="68"/>
-      <c r="F103" s="76"/>
-      <c r="G103" s="77"/>
-      <c r="H103" s="73"/>
-    </row>
-    <row r="104" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B104" s="12" t="s">
+      <c r="D102" s="97"/>
+      <c r="F102" s="65"/>
+      <c r="G102" s="66"/>
+      <c r="H102" s="62"/>
+    </row>
+    <row r="103" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B103" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C104" s="23">
+      <c r="C103" s="23">
         <v>0</v>
       </c>
-      <c r="D104" s="69"/>
-    </row>
-    <row r="105" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="D103" s="98"/>
+    </row>
+    <row r="104" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B105" s="92" t="s">
+        <v>0</v>
+      </c>
+      <c r="C105" s="93"/>
+      <c r="D105" s="47" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B106" s="63" t="s">
-        <v>0</v>
-      </c>
-      <c r="C106" s="64"/>
-      <c r="D106" s="47" t="s">
-        <v>16</v>
-      </c>
+      <c r="B106" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D106" s="83"/>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>1</v>
+        <v>63</v>
       </c>
       <c r="C107" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D107" s="92"/>
+        <v>73</v>
+      </c>
+      <c r="D107" s="84"/>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C108" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D108" s="93"/>
+        <v>68</v>
+      </c>
+      <c r="D108" s="84"/>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C109" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D109" s="93"/>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B110" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C110" s="13">
+      <c r="C109" s="13">
         <v>14.2</v>
       </c>
-      <c r="D110" s="93"/>
-    </row>
-    <row r="111" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B111" s="4" t="s">
+      <c r="D109" s="84"/>
+    </row>
+    <row r="110" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B110" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C111" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D111" s="94"/>
-    </row>
-    <row r="112" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C110" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D110" s="85"/>
+    </row>
+    <row r="111" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B112" s="104" t="s">
+        <v>60</v>
+      </c>
+      <c r="C112" s="105"/>
+      <c r="D112" s="53" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" s="107" t="s">
-        <v>62</v>
-      </c>
-      <c r="C113" s="108"/>
-      <c r="D113" s="55" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B114" s="74"/>
-      <c r="C114" s="75"/>
-      <c r="D114" s="72"/>
-    </row>
-    <row r="115" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B115" s="76"/>
-      <c r="C115" s="77"/>
-      <c r="D115" s="73"/>
+      <c r="B113" s="63"/>
+      <c r="C113" s="64"/>
+      <c r="D113" s="61"/>
+    </row>
+    <row r="114" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B114" s="65"/>
+      <c r="C114" s="66"/>
+      <c r="D114" s="62"/>
+    </row>
+    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="K116" s="24"/>
+      <c r="L116" s="24"/>
+      <c r="N116"/>
+      <c r="O116"/>
     </row>
     <row r="117" spans="2:15" x14ac:dyDescent="0.25">
       <c r="K117" s="24"/>
@@ -4344,69 +4369,63 @@
       <c r="N121"/>
       <c r="O121"/>
     </row>
-    <row r="122" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K122" s="24"/>
-      <c r="L122" s="24"/>
-      <c r="N122"/>
-      <c r="O122"/>
-    </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="H95:H99"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="H90:H92"/>
-    <mergeCell ref="B94:C94"/>
-    <mergeCell ref="D95:D99"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="B114:C115"/>
-    <mergeCell ref="D114:D115"/>
-    <mergeCell ref="F102:G103"/>
-    <mergeCell ref="H102:H103"/>
-    <mergeCell ref="B106:C106"/>
-    <mergeCell ref="D107:D111"/>
-    <mergeCell ref="D102:D104"/>
-    <mergeCell ref="D83:D87"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="D90:D92"/>
-    <mergeCell ref="F94:G94"/>
-    <mergeCell ref="H83:H87"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="B82:C82"/>
-    <mergeCell ref="B75:C75"/>
-    <mergeCell ref="D76:D80"/>
-    <mergeCell ref="F82:G82"/>
-    <mergeCell ref="F75:G75"/>
-    <mergeCell ref="H76:H80"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H72:H73"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="F52:F54"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F61:F63"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="F67:F69"/>
-    <mergeCell ref="F45:F49"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F20:F24"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="F28:F32"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F35:F37"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="D75:D79"/>
+    <mergeCell ref="H75:H79"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="F60:F62"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="F56:F57"/>
+    <mergeCell ref="F66:F68"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="H82:H86"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="B81:C81"/>
+    <mergeCell ref="B113:C114"/>
+    <mergeCell ref="D113:D114"/>
+    <mergeCell ref="F101:G102"/>
+    <mergeCell ref="H101:H102"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="D106:D110"/>
+    <mergeCell ref="D101:D103"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="H89:H91"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="D94:D98"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="F100:G100"/>
+    <mergeCell ref="F93:G93"/>
+    <mergeCell ref="F81:G81"/>
+    <mergeCell ref="F74:G74"/>
+    <mergeCell ref="H94:H98"/>
+    <mergeCell ref="D82:D86"/>
+    <mergeCell ref="F44:F48"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F34:F36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4417,43 +4436,43 @@
           <x14:formula1>
             <xm:f>'___Dropdown values'!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E4 E10 E58 C73:C74 G73:G74</xm:sqref>
+          <xm:sqref>E4 E10 E57 C72:C73 G72:G73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C6B8CA4-BBDF-4720-83DB-EEB75CAAC296}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$B$10:$B$17</xm:f>
           </x14:formula1>
-          <xm:sqref>E14 E29 E46 C84 G84 C96 C108 G96 C77 G77</xm:sqref>
+          <xm:sqref>E14 E28 E45 C83 G83 C95 C107 G95 C76 G76</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{934B1DA1-8C91-4057-973F-82597951F8B7}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$F$5:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D12:E12 D27:E27 D44:E44 B82:C82 F82:G82 B94:C94 B106:C106 F94:G94 B75:C75 F75:G75</xm:sqref>
+          <xm:sqref>D12:E12 D26:E26 D43:E43 B81:C81 F81:G81 B93:C93 B105:C105 F93:G93 B74:C74 F74:G74</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1EA7122-9BB0-47F3-A320-6D1AE93FB4E0}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$D$10:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E17 E40 G80 C80 G99 C111 C99 G87 C87 E49 E32</xm:sqref>
+          <xm:sqref>E17 E39 G79 C79 G98 C110 C98 G86 C86 E48 E31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6BE6F825-91BE-4CEC-9D14-5710077D0618}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$B$20:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>E15 C78 G97 C109 C97 G85 E30 E47 C85 G78</xm:sqref>
+          <xm:sqref>E15 C77 G96 C108 C96 G84 E29 E46 C84 G77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F317EFE0-6C20-4FA6-8CE8-F5ABF95CC729}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$K$5:$K$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D34:E34 D51:E51 B89:C89 F89:G89 B101:C101</xm:sqref>
+          <xm:sqref>D33:E33 D50:E50 B88:C88 F88:G88 B100:C100</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{345D99D0-6529-4A67-8275-A029C65E5115}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$H$5:$H$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D60:E60</xm:sqref>
+          <xm:sqref>D59:E59</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{998DE1DC-BE8F-41C0-A011-BA46036902B2}">
           <x14:formula1>
@@ -4465,19 +4484,19 @@
           <x14:formula1>
             <xm:f>'___Dropdown values'!$I$5:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D39:E39</xm:sqref>
+          <xm:sqref>D38:E38</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C124AD9A-B163-4E82-86EB-DE4F7DADE970}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$D$4:$D$7</xm:f>
           </x14:formula1>
-          <xm:sqref>E64</xm:sqref>
+          <xm:sqref>E63</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D33A016A-FF6B-485D-892B-56B9C722EB80}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$D$4:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>E63</xm:sqref>
+          <xm:sqref>E62</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4490,8 +4509,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4517,7 +4536,7 @@
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -4526,16 +4545,16 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
         <v>52</v>
       </c>
-      <c r="F1" t="s">
-        <v>54</v>
-      </c>
       <c r="G1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4544,7 +4563,6 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B5" si="1">A2</f>
         <v>1</v>
       </c>
       <c r="C2" t="s">
@@ -4560,7 +4578,7 @@
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -4572,7 +4590,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="B3:B5" si="1">A3</f>
         <v>2</v>
       </c>
       <c r="C3" t="s">
@@ -4588,7 +4606,7 @@
         <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H3">
         <v>10</v>
@@ -4616,7 +4634,7 @@
         <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H4">
         <v>15</v>
@@ -4644,7 +4662,7 @@
         <v>26</v>
       </c>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H5">
         <v>15</v>
@@ -5840,18 +5858,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5874,18 +5892,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158388FD-FCB9-4D40-8807-AFB22AE8C172}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46E792D2-13D9-445F-AE7B-CF179A33399C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158388FD-FCB9-4D40-8807-AFB22AE8C172}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added step checks to ensure step is actually used before we run the PreRun Methods. Updated Hamilton method accordingly.
</commit_message>
<xml_diff>
--- a/Method Maker1.xlsx
+++ b/Method Maker1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\program files (x86)\hamilton\bareb\script\hamiltonmethodmaker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\HAMILTON\BAREB\Script\HamiltonMethodMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4901BC-71FF-469B-8169-3CF9065C6773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4368BA-AF9B-46D9-ABA1-740A3A2954FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{132869CD-930B-4C8C-A6DF-075DCD3A8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="___Dropdown values" sheetId="4" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="91">
   <si>
     <t>Liquid Transfer</t>
   </si>
@@ -161,9 +161,6 @@
     <t>Equilibration Buffer</t>
   </si>
   <si>
-    <t>Sample Volume (uL)</t>
-  </si>
-  <si>
     <t>Source</t>
   </si>
   <si>
@@ -191,15 +188,6 @@
     <t>_Conc</t>
   </si>
   <si>
-    <t>1M IAA</t>
-  </si>
-  <si>
-    <t>Digestion Pathway</t>
-  </si>
-  <si>
-    <t>PNGaseF</t>
-  </si>
-  <si>
     <t>This plate is always included. Method workflow requires the samples start in a 96well plate (For Now)</t>
   </si>
   <si>
@@ -266,39 +254,9 @@
     <t>Denaturant</t>
   </si>
   <si>
-    <t>100mM Tris pH8.2</t>
-  </si>
-  <si>
     <t>Desalting</t>
   </si>
   <si>
-    <t>0.2 mg/mL Trypsin in 100mM Tris pH8.2</t>
-  </si>
-  <si>
-    <t>50% TFA</t>
-  </si>
-  <si>
-    <t>1st Pipetting Step</t>
-  </si>
-  <si>
-    <t>Liquid 1</t>
-  </si>
-  <si>
-    <t>Liquid 2</t>
-  </si>
-  <si>
-    <t>Liquid 3</t>
-  </si>
-  <si>
-    <t>Test Message</t>
-  </si>
-  <si>
-    <t>This is a Test Message.\nThank you for reading!</t>
-  </si>
-  <si>
-    <t>Volumes</t>
-  </si>
-  <si>
     <t>SizeX:100</t>
   </si>
   <si>
@@ -312,6 +270,45 @@
   </si>
   <si>
     <t>Source Plate</t>
+  </si>
+  <si>
+    <t>300mM DTT in Denaturation Buffer</t>
+  </si>
+  <si>
+    <t>Denaturation Buffer</t>
+  </si>
+  <si>
+    <t>500mM IAA in Denaturation Buffer</t>
+  </si>
+  <si>
+    <t>Digestion Buffer</t>
+  </si>
+  <si>
+    <t>Desalting Complete</t>
+  </si>
+  <si>
+    <t>Desalted Concentration</t>
+  </si>
+  <si>
+    <t>Hello. Desalting is complete. Please measure each sample with A280 then enter concentration in the Desalted Concentration column</t>
+  </si>
+  <si>
+    <t>1.0 mg/mL Trypsin in 500mM Acetic Acid</t>
+  </si>
+  <si>
+    <t>10% TFA</t>
+  </si>
+  <si>
+    <t>Pathway</t>
+  </si>
+  <si>
+    <t>500mM DTT</t>
+  </si>
+  <si>
+    <t>500mM TCEP</t>
+  </si>
+  <si>
+    <t>Digestion</t>
   </si>
 </sst>
 </file>
@@ -669,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -760,9 +757,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -770,180 +764,179 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -958,68 +951,29 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="192">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="186">
     <dxf>
       <fill>
         <patternFill>
@@ -2659,58 +2613,58 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" s="60" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="49" t="s">
-        <v>87</v>
-      </c>
-      <c r="F4" s="43" t="s">
+      <c r="D4" s="46" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="G4" s="43" t="s">
+      <c r="G4" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="43" t="s">
+      <c r="H4" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="I4" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="43" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" s="43" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="43" t="s">
-        <v>64</v>
+      <c r="J4" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="K4" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="42" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" s="49" t="s">
-        <v>88</v>
+        <v>61</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>74</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -2725,20 +2679,20 @@
         <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="K5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="46"/>
       <c r="F6" t="s">
         <v>30</v>
       </c>
@@ -2752,63 +2706,63 @@
         <v>33</v>
       </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="49"/>
+        <v>63</v>
+      </c>
+      <c r="D7" s="46"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="43" t="s">
-        <v>63</v>
+      <c r="B9" s="42" t="s">
+        <v>59</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -2822,18 +2776,18 @@
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
-        <v>61</v>
+      <c r="B19" s="42" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2851,7 +2805,7 @@
   <dimension ref="C2:Q21"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="C13" sqref="C13:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,31 +2832,31 @@
   <sheetData>
     <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="70"/>
-      <c r="E3" s="53" t="s">
+      <c r="D3" s="62"/>
+      <c r="E3" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="72"/>
+      <c r="H3" s="75"/>
       <c r="I3" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="75" t="s">
+      <c r="K3" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="76"/>
+      <c r="L3" s="79"/>
       <c r="M3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="P3" s="68"/>
+      <c r="O3" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="73"/>
       <c r="Q3" s="28" t="s">
         <v>16</v>
       </c>
@@ -2912,74 +2866,74 @@
         <v>1</v>
       </c>
       <c r="D4" s="34"/>
-      <c r="E4" s="61"/>
+      <c r="E4" s="66"/>
       <c r="G4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H4" s="15"/>
-      <c r="I4" s="86"/>
+      <c r="I4" s="89"/>
       <c r="K4" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="20"/>
-      <c r="M4" s="89"/>
+      <c r="M4" s="92"/>
       <c r="O4" s="11" t="s">
         <v>13</v>
       </c>
       <c r="P4" s="22"/>
-      <c r="Q4" s="96"/>
+      <c r="Q4" s="58"/>
     </row>
     <row r="5" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="48" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="33"/>
-      <c r="E5" s="62"/>
+      <c r="E5" s="67"/>
       <c r="G5" s="7" t="s">
         <v>3</v>
       </c>
       <c r="H5" s="15"/>
-      <c r="I5" s="87"/>
+      <c r="I5" s="90"/>
       <c r="K5" s="5" t="s">
         <v>40</v>
       </c>
       <c r="L5" s="20"/>
-      <c r="M5" s="90"/>
+      <c r="M5" s="93"/>
       <c r="O5" s="11" t="s">
         <v>9</v>
       </c>
       <c r="P5" s="22"/>
-      <c r="Q5" s="97"/>
+      <c r="Q5" s="59"/>
     </row>
     <row r="6" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="H6" s="15"/>
-      <c r="I6" s="87"/>
+      <c r="I6" s="90"/>
       <c r="K6" s="6" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="L6" s="21"/>
-      <c r="M6" s="91"/>
+      <c r="M6" s="94"/>
       <c r="O6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="P6" s="23"/>
-      <c r="Q6" s="98"/>
+      <c r="Q6" s="60"/>
     </row>
     <row r="7" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G7" s="7" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="15"/>
-      <c r="I7" s="87"/>
+      <c r="I7" s="90"/>
     </row>
     <row r="8" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="73" t="s">
+      <c r="C8" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="74"/>
+      <c r="D8" s="77"/>
       <c r="E8" s="25" t="s">
         <v>16</v>
       </c>
@@ -2987,19 +2941,19 @@
         <v>11</v>
       </c>
       <c r="H8" s="16"/>
-      <c r="I8" s="88"/>
+      <c r="I8" s="91"/>
     </row>
     <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="18"/>
-      <c r="E9" s="77"/>
-      <c r="K9" s="69" t="s">
+      <c r="E9" s="80"/>
+      <c r="K9" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="70"/>
-      <c r="M9" s="45" t="s">
+      <c r="L9" s="62"/>
+      <c r="M9" s="44" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3008,124 +2962,118 @@
         <v>38</v>
       </c>
       <c r="D10" s="18"/>
-      <c r="E10" s="78"/>
-      <c r="G10" s="92" t="s">
+      <c r="E10" s="81"/>
+      <c r="G10" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="93"/>
+      <c r="H10" s="96"/>
       <c r="I10" s="29" t="s">
         <v>16</v>
       </c>
       <c r="K10" s="31" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="L10" s="32"/>
-      <c r="M10" s="80"/>
+      <c r="M10" s="83"/>
     </row>
     <row r="11" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="10" t="s">
         <v>39</v>
       </c>
       <c r="D11" s="19"/>
-      <c r="E11" s="79"/>
+      <c r="E11" s="82"/>
       <c r="G11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H11" s="13"/>
-      <c r="I11" s="83"/>
+      <c r="I11" s="86"/>
       <c r="K11" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="L11" s="32"/>
-      <c r="M11" s="81"/>
+      <c r="L11" s="111"/>
+      <c r="M11" s="84"/>
     </row>
     <row r="12" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G12" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H12" s="13"/>
-      <c r="I12" s="84"/>
+      <c r="I12" s="87"/>
       <c r="K12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="82"/>
+      <c r="L12" s="110"/>
+      <c r="M12" s="85"/>
     </row>
     <row r="13" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C13" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="70"/>
-      <c r="E13" s="44" t="s">
+      <c r="C13" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="62"/>
+      <c r="E13" s="43" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H13" s="13"/>
-      <c r="I13" s="84"/>
+      <c r="I13" s="87"/>
     </row>
     <row r="14" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="63"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="61"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="66"/>
       <c r="G14" s="3" t="s">
         <v>12</v>
       </c>
       <c r="H14" s="13"/>
-      <c r="I14" s="84"/>
+      <c r="I14" s="87"/>
     </row>
     <row r="15" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="65"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="62"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="67"/>
       <c r="G15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="85"/>
+      <c r="I15" s="88"/>
     </row>
     <row r="17" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G18" s="94" t="s">
-        <v>48</v>
-      </c>
-      <c r="H18" s="95"/>
+      <c r="G18" s="56" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="57"/>
       <c r="I18" s="36" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G19" s="58" t="s">
-        <v>91</v>
-      </c>
-      <c r="H19" s="59"/>
-      <c r="I19" s="99"/>
+      <c r="G19" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="50"/>
+      <c r="I19" s="63"/>
     </row>
     <row r="20" spans="7:9" x14ac:dyDescent="0.25">
       <c r="G20" s="37" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="H20" s="38"/>
-      <c r="I20" s="100"/>
+      <c r="I20" s="64"/>
     </row>
     <row r="21" spans="7:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G21" s="39" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="H21" s="40"/>
-      <c r="I21" s="101"/>
+      <c r="I21" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="Q4:Q6"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="I19:I21"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E14:E15"/>
     <mergeCell ref="C14:D15"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="C3:D3"/>
@@ -3139,6 +3087,12 @@
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="Q4:Q6"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="I19:I21"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E14:E15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3208,10 +3162,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88364F8-85B5-4C5D-8958-0F9155266F29}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="B1:O121"/>
+  <dimension ref="D1:O103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C26" sqref="A26:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3220,7 +3174,7 @@
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="43" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="55.140625" customWidth="1"/>
     <col min="7" max="7" width="43" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -3232,10 +3186,10 @@
   <sheetData>
     <row r="1" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="70"/>
+      <c r="E2" s="62"/>
       <c r="F2" s="30" t="s">
         <v>16</v>
       </c>
@@ -3247,8 +3201,8 @@
       <c r="E3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="61" t="s">
-        <v>54</v>
+      <c r="F3" s="66" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3258,20 +3212,20 @@
       <c r="E4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="62"/>
+      <c r="F4" s="67"/>
     </row>
     <row r="6" spans="4:15" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="114" t="s">
+      <c r="D6" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="114"/>
+      <c r="E6" s="103"/>
     </row>
     <row r="7" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D8" s="104" t="s">
+      <c r="D8" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="105"/>
+      <c r="E8" s="102"/>
       <c r="F8" s="41" t="s">
         <v>16</v>
       </c>
@@ -3281,9 +3235,9 @@
         <v>1</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="112"/>
+        <v>48</v>
+      </c>
+      <c r="F9" s="99"/>
     </row>
     <row r="10" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="1" t="s">
@@ -3292,7 +3246,7 @@
       <c r="E10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="113"/>
+      <c r="F10" s="100"/>
     </row>
     <row r="11" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I11" s="24"/>
@@ -3301,11 +3255,11 @@
       <c r="O11"/>
     </row>
     <row r="12" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D12" s="102" t="s">
+      <c r="D12" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="103"/>
-      <c r="F12" s="47" t="s">
+      <c r="E12" s="98"/>
+      <c r="F12" s="45" t="s">
         <v>16</v>
       </c>
       <c r="N12"/>
@@ -3315,22 +3269,21 @@
       <c r="D13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="13" t="str">
-        <f>Worklist!G1</f>
-        <v>1st Pipetting Step</v>
-      </c>
-      <c r="F13" s="83"/>
+      <c r="E13" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="86"/>
       <c r="N13"/>
       <c r="O13"/>
     </row>
     <row r="14" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D14" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="84"/>
+        <v>71</v>
+      </c>
+      <c r="F14" s="87"/>
       <c r="K14" s="24"/>
       <c r="L14" s="24"/>
       <c r="N14"/>
@@ -3338,12 +3291,12 @@
     </row>
     <row r="15" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="84"/>
+        <v>64</v>
+      </c>
+      <c r="F15" s="87"/>
       <c r="K15" s="24"/>
       <c r="L15" s="24"/>
       <c r="N15"/>
@@ -3353,10 +3306,10 @@
       <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16" s="84"/>
+      <c r="E16" s="13">
+        <v>86</v>
+      </c>
+      <c r="F16" s="87"/>
       <c r="K16" s="24"/>
       <c r="L16" s="24"/>
       <c r="N16"/>
@@ -3364,12 +3317,12 @@
     </row>
     <row r="17" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="85"/>
+      <c r="F17" s="88"/>
       <c r="K17" s="24"/>
       <c r="L17" s="24"/>
       <c r="N17"/>
@@ -3382,10 +3335,10 @@
       <c r="O18"/>
     </row>
     <row r="19" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D19" s="71" t="s">
+      <c r="D19" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="72"/>
+      <c r="E19" s="109"/>
       <c r="F19" s="26" t="s">
         <v>16</v>
       </c>
@@ -3396,12 +3349,12 @@
     </row>
     <row r="20" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D20" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F20" s="86"/>
+      <c r="F20" s="89"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24"/>
       <c r="N20"/>
@@ -3414,7 +3367,7 @@
       <c r="E21" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="87"/>
+      <c r="F21" s="90"/>
       <c r="K21" s="24"/>
       <c r="L21" s="24"/>
       <c r="N21"/>
@@ -3428,7 +3381,7 @@
         <f>Worklist!E1</f>
         <v>_Conc</v>
       </c>
-      <c r="F22" s="87"/>
+      <c r="F22" s="90"/>
       <c r="K22" s="24"/>
       <c r="L22" s="24"/>
       <c r="N22"/>
@@ -3441,7 +3394,7 @@
       <c r="E23" s="15">
         <v>10</v>
       </c>
-      <c r="F23" s="87"/>
+      <c r="F23" s="90"/>
       <c r="K23" s="24"/>
       <c r="L23" s="24"/>
       <c r="N23"/>
@@ -3452,9 +3405,9 @@
         <v>11</v>
       </c>
       <c r="E24" s="16">
-        <v>50</v>
-      </c>
-      <c r="F24" s="88"/>
+        <v>10</v>
+      </c>
+      <c r="F24" s="91"/>
       <c r="K24" s="24"/>
       <c r="L24" s="24"/>
       <c r="N24"/>
@@ -3467,1036 +3420,723 @@
       <c r="O25"/>
     </row>
     <row r="26" spans="4:15" x14ac:dyDescent="0.25">
-      <c r="D26" s="102" t="s">
+      <c r="D26" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="103"/>
-      <c r="F26" s="47" t="s">
+      <c r="E26" s="96"/>
+      <c r="F26" s="51" t="s">
         <v>16</v>
       </c>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="N26"/>
+      <c r="O26"/>
     </row>
     <row r="27" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D27" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" s="83"/>
+      <c r="E27" s="13" t="str">
+        <f>Worklist!H1</f>
+        <v>Reductant</v>
+      </c>
+      <c r="F27" s="86"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="N27"/>
+      <c r="O27"/>
     </row>
     <row r="28" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D28" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="84"/>
+        <v>66</v>
+      </c>
+      <c r="F28" s="87"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="N28"/>
+      <c r="O28"/>
     </row>
     <row r="29" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D29" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="84"/>
+        <v>64</v>
+      </c>
+      <c r="F29" s="87"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="N29"/>
+      <c r="O29"/>
     </row>
     <row r="30" spans="4:15" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="13">
-        <v>5</v>
-      </c>
-      <c r="F30" s="84"/>
+        <v>4</v>
+      </c>
+      <c r="F30" s="87"/>
     </row>
     <row r="31" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D31" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E31" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="85"/>
+      <c r="F31" s="88"/>
     </row>
     <row r="32" spans="4:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D33" s="106" t="s">
-        <v>43</v>
-      </c>
-      <c r="E33" s="107"/>
-      <c r="F33" s="28" t="s">
+      <c r="D33" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="96"/>
+      <c r="F33" s="51" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="34" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D34" s="11" t="s">
+      <c r="D34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="86"/>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" s="87"/>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F36" s="87"/>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" s="13">
+        <v>3.33</v>
+      </c>
+      <c r="F37" s="87"/>
+    </row>
+    <row r="38" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F38" s="88"/>
+    </row>
+    <row r="39" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="73"/>
+      <c r="F40" s="53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="22">
-        <v>37</v>
-      </c>
-      <c r="F34" s="96"/>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="11" t="s">
+      <c r="E41" s="22">
+        <v>30</v>
+      </c>
+      <c r="F41" s="58"/>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D42" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="22">
-        <v>60</v>
-      </c>
-      <c r="F35" s="97"/>
-    </row>
-    <row r="36" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="12" t="s">
+      <c r="E42" s="22">
+        <v>30</v>
+      </c>
+      <c r="F42" s="59"/>
+    </row>
+    <row r="43" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E36" s="23">
+      <c r="E43" s="23">
         <v>0</v>
       </c>
-      <c r="F36" s="98"/>
-    </row>
-    <row r="37" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D38" s="69" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="70"/>
-      <c r="F38" s="45" t="s">
+      <c r="F43" s="60"/>
+    </row>
+    <row r="44" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D45" s="95" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="96"/>
+      <c r="F45" s="51" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D39" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="E39" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="F39" s="80"/>
-    </row>
-    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D40" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F40" s="81"/>
-    </row>
-    <row r="41" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="F41" s="82"/>
-    </row>
-    <row r="42" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D43" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="E43" s="103"/>
-      <c r="F43" s="47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D44" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F44" s="83"/>
-    </row>
-    <row r="45" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D45" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E45" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F45" s="84"/>
     </row>
     <row r="46" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D46" s="3" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F46" s="84"/>
+        <v>80</v>
+      </c>
+      <c r="F46" s="86"/>
     </row>
     <row r="47" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D47" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" s="87"/>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D48" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F48" s="87"/>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D49" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E47" s="13">
-        <v>301</v>
-      </c>
-      <c r="F47" s="84"/>
-    </row>
-    <row r="48" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D48" s="4" t="s">
+      <c r="E49" s="13">
+        <v>5</v>
+      </c>
+      <c r="F49" s="87"/>
+    </row>
+    <row r="50" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D50" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E48" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="F48" s="85"/>
-    </row>
-    <row r="49" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D50" s="106" t="s">
-        <v>43</v>
-      </c>
-      <c r="E50" s="107"/>
-      <c r="F50" s="28" t="s">
+      <c r="F50" s="88"/>
+    </row>
+    <row r="51" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D52" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E52" s="73"/>
+      <c r="F52" s="53" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D51" s="11" t="s">
+    <row r="53" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D53" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="F51" s="96"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D52" s="11" t="s">
+      <c r="E53" s="22">
+        <v>25</v>
+      </c>
+      <c r="F53" s="58"/>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="22">
+      <c r="E54" s="22">
+        <v>30</v>
+      </c>
+      <c r="F54" s="59"/>
+    </row>
+    <row r="55" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D55" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E55" s="23">
+        <v>0</v>
+      </c>
+      <c r="F55" s="60"/>
+    </row>
+    <row r="56" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="101" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="102"/>
+      <c r="F57" s="52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D58" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>72</v>
+      </c>
+      <c r="F58" s="99"/>
+    </row>
+    <row r="59" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D59" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F59" s="100"/>
+    </row>
+    <row r="60" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D61" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="107"/>
+      <c r="F61" s="54" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D62" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E62" s="20" t="str">
+        <f>E9</f>
+        <v>Denaturation</v>
+      </c>
+      <c r="F62" s="92"/>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D63" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E63" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="F63" s="93"/>
+    </row>
+    <row r="64" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D64" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F64" s="94"/>
+    </row>
+    <row r="65" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D66" s="101" t="s">
+        <v>22</v>
+      </c>
+      <c r="E66" s="102"/>
+      <c r="F66" s="44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="67" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D67" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E67" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F67" s="83"/>
+    </row>
+    <row r="68" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D68" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F68" s="84"/>
+    </row>
+    <row r="69" spans="4:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E69" s="110" t="s">
+        <v>84</v>
+      </c>
+      <c r="F69" s="85"/>
+    </row>
+    <row r="70" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D70" s="24"/>
+      <c r="E70" s="112"/>
+      <c r="F70" s="113"/>
+    </row>
+    <row r="71" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D71" s="101" t="s">
+        <v>2</v>
+      </c>
+      <c r="E71" s="102"/>
+      <c r="F71" s="52" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D72" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E72" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="F72" s="99"/>
+    </row>
+    <row r="73" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F73" s="100"/>
+    </row>
+    <row r="74" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D75" s="108" t="s">
+        <v>17</v>
+      </c>
+      <c r="E75" s="109"/>
+      <c r="F75" s="26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D76" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="F76" s="89"/>
+    </row>
+    <row r="77" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D77" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="F77" s="90"/>
+    </row>
+    <row r="78" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D78" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="15" t="str">
+        <f>Worklist!F1</f>
+        <v>Desalted Concentration</v>
+      </c>
+      <c r="F78" s="90"/>
+    </row>
+    <row r="79" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D79" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E79" s="15">
+        <v>10</v>
+      </c>
+      <c r="F79" s="90"/>
+    </row>
+    <row r="80" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D80" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="16">
+        <v>10</v>
+      </c>
+      <c r="F80" s="91"/>
+    </row>
+    <row r="81" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D82" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="E82" s="98"/>
+      <c r="F82" s="51" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D83" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F83" s="86"/>
+    </row>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D84" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F84" s="87"/>
+    </row>
+    <row r="85" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D85" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F85" s="87"/>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" s="13">
+        <v>3.2</v>
+      </c>
+      <c r="F86" s="87"/>
+    </row>
+    <row r="87" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D87" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F87" s="88"/>
+    </row>
+    <row r="88" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="89" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D89" s="104" t="s">
+        <v>42</v>
+      </c>
+      <c r="E89" s="105"/>
+      <c r="F89" s="53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D90" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E90" s="22">
+        <v>37</v>
+      </c>
+      <c r="F90" s="58"/>
+    </row>
+    <row r="91" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D91" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" s="22">
         <v>60</v>
       </c>
-      <c r="F52" s="97"/>
-    </row>
-    <row r="53" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D53" s="12" t="s">
+      <c r="F91" s="59"/>
+    </row>
+    <row r="92" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D92" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E53" s="23">
+      <c r="E92" s="23">
         <v>0</v>
       </c>
-      <c r="F53" s="98"/>
-    </row>
-    <row r="54" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D55" s="104" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55" s="105"/>
-      <c r="F55" s="48" t="s">
+      <c r="F92" s="60"/>
+    </row>
+    <row r="93" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D94" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="E94" s="98"/>
+      <c r="F94" s="51" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="31" t="s">
+    <row r="95" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D95" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E56" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="F56" s="61"/>
-    </row>
-    <row r="57" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D57" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E57" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="F57" s="62"/>
-    </row>
-    <row r="58" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D59" s="108" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="109"/>
-      <c r="F59" s="46" t="s">
+      <c r="E95" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="F95" s="86"/>
+    </row>
+    <row r="96" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D96" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F96" s="87"/>
+    </row>
+    <row r="97" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D97" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F97" s="87"/>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D98" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="13">
+        <v>1.7</v>
+      </c>
+      <c r="F98" s="87"/>
+    </row>
+    <row r="99" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D99" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E99" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="F99" s="88"/>
+    </row>
+    <row r="100" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D101" s="101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E101" s="102"/>
+      <c r="F101" s="52" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F60" s="89"/>
-    </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D61" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="F61" s="90"/>
-    </row>
-    <row r="62" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D62" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E62" s="21" t="s">
-        <v>88</v>
-      </c>
-      <c r="F62" s="91"/>
-    </row>
-    <row r="63" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D63" s="55"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="57"/>
-    </row>
-    <row r="64" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D65" s="110" t="s">
-        <v>4</v>
-      </c>
-      <c r="E65" s="111"/>
-      <c r="F65" s="25" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D66" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E66" s="18" t="str">
-        <f>Worklist!F1</f>
-        <v>Digestion Pathway</v>
-      </c>
-      <c r="F66" s="77"/>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D67" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="E67" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F67" s="78"/>
-    </row>
-    <row r="68" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D68" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E68" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="F68" s="79"/>
-    </row>
-    <row r="69" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="69" t="s">
-        <v>2</v>
-      </c>
-      <c r="C70" s="70"/>
-      <c r="D70" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="F70" s="104" t="s">
-        <v>2</v>
-      </c>
-      <c r="G70" s="105"/>
-      <c r="H70" s="48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="34" t="s">
-        <v>25</v>
-      </c>
-      <c r="D71" s="61"/>
-      <c r="F71" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="G71" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="H71" s="61"/>
-    </row>
-    <row r="72" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B72" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C72" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="D72" s="62"/>
-      <c r="F72" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G72" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="H72" s="62"/>
-    </row>
-    <row r="73" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B73" s="24"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="52"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="51"/>
-      <c r="H73" s="52"/>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="C74" s="93"/>
-      <c r="D74" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="F74" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="G74" s="103"/>
-      <c r="H74" s="47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C75" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="D75" s="83"/>
-      <c r="F75" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G75" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="H75" s="83"/>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C76" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D76" s="84"/>
-      <c r="F76" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G76" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H76" s="84"/>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C77" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D77" s="84"/>
-      <c r="F77" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G77" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H77" s="84"/>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C78" s="13">
-        <v>250</v>
-      </c>
-      <c r="D78" s="84"/>
-      <c r="F78" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" s="13">
-        <v>250</v>
-      </c>
-      <c r="H78" s="84"/>
-    </row>
-    <row r="79" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D79" s="85"/>
-      <c r="F79" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G79" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="H79" s="85"/>
-    </row>
-    <row r="80" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="93"/>
-      <c r="D81" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="F81" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="G81" s="103"/>
-      <c r="H81" s="47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C82" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="D82" s="83"/>
-      <c r="F82" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G82" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="H82" s="83"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C83" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D83" s="84"/>
-      <c r="F83" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G83" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H83" s="84"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C84" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D84" s="84"/>
-      <c r="F84" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G84" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H84" s="84"/>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C85" s="13">
-        <v>3.6</v>
-      </c>
-      <c r="D85" s="84"/>
-      <c r="F85" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G85" s="13">
-        <v>30</v>
-      </c>
-      <c r="H85" s="84"/>
-    </row>
-    <row r="86" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B86" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C86" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D86" s="85"/>
-      <c r="F86" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G86" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H86" s="85"/>
-    </row>
-    <row r="87" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="C88" s="68"/>
-      <c r="D88" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F88" s="106" t="s">
-        <v>43</v>
-      </c>
-      <c r="G88" s="107"/>
-      <c r="H88" s="28" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C89" s="22">
-        <v>37</v>
-      </c>
-      <c r="D89" s="96"/>
-      <c r="F89" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G89" s="22">
-        <v>37</v>
-      </c>
-      <c r="H89" s="96"/>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C90" s="22">
-        <f>18*60</f>
-        <v>1080</v>
-      </c>
-      <c r="D90" s="97"/>
-      <c r="F90" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G90" s="22">
-        <v>5000</v>
-      </c>
-      <c r="H90" s="97"/>
-    </row>
-    <row r="91" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B91" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C91" s="23">
-        <v>0</v>
-      </c>
-      <c r="D91" s="98"/>
-      <c r="F91" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G91" s="23">
-        <v>0</v>
-      </c>
-      <c r="H91" s="98"/>
-    </row>
-    <row r="92" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="C93" s="93"/>
-      <c r="D93" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="F93" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="G93" s="103"/>
-      <c r="H93" s="47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C94" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="D94" s="83"/>
-      <c r="F94" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G94" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="H94" s="83"/>
-    </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C95" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D95" s="84"/>
-      <c r="F95" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G95" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="H95" s="84"/>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C96" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="D96" s="84"/>
-      <c r="F96" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G96" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="H96" s="84"/>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C97" s="50">
-        <v>30</v>
-      </c>
-      <c r="D97" s="84"/>
-      <c r="F97" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G97" s="13">
-        <v>14.2</v>
-      </c>
-      <c r="H97" s="84"/>
-    </row>
-    <row r="98" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B98" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C98" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D98" s="85"/>
-      <c r="F98" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G98" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H98" s="85"/>
-    </row>
-    <row r="99" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="67" t="s">
-        <v>43</v>
-      </c>
-      <c r="C100" s="68"/>
-      <c r="D100" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="F100" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="G100" s="105"/>
-      <c r="H100" s="48" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C101" s="22">
-        <v>37</v>
-      </c>
-      <c r="D101" s="96"/>
-      <c r="F101" s="63"/>
-      <c r="G101" s="64"/>
-      <c r="H101" s="61"/>
-    </row>
-    <row r="102" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B102" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C102" s="22">
-        <f>60*4</f>
-        <v>240</v>
-      </c>
-      <c r="D102" s="97"/>
-      <c r="F102" s="65"/>
-      <c r="G102" s="66"/>
-      <c r="H102" s="62"/>
-    </row>
-    <row r="103" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B103" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C103" s="23">
-        <v>0</v>
-      </c>
-      <c r="D103" s="98"/>
-    </row>
-    <row r="104" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B105" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="C105" s="93"/>
-      <c r="D105" s="47" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B106" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C106" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D106" s="83"/>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B107" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C107" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D107" s="84"/>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B108" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C108" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="D108" s="84"/>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C109" s="13">
-        <v>14.2</v>
-      </c>
-      <c r="D109" s="84"/>
-    </row>
-    <row r="110" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B110" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D110" s="85"/>
-    </row>
-    <row r="111" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B112" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="C112" s="105"/>
-      <c r="D112" s="53" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B113" s="63"/>
-      <c r="C113" s="64"/>
-      <c r="D113" s="61"/>
-    </row>
-    <row r="114" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B114" s="65"/>
-      <c r="C114" s="66"/>
-      <c r="D114" s="62"/>
-    </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K116" s="24"/>
-      <c r="L116" s="24"/>
-      <c r="N116"/>
-      <c r="O116"/>
-    </row>
-    <row r="117" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K117" s="24"/>
-      <c r="L117" s="24"/>
-      <c r="N117"/>
-      <c r="O117"/>
-    </row>
-    <row r="118" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K118" s="24"/>
-      <c r="L118" s="24"/>
-      <c r="N118"/>
-      <c r="O118"/>
-    </row>
-    <row r="119" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K119" s="24"/>
-      <c r="L119" s="24"/>
-      <c r="N119"/>
-      <c r="O119"/>
-    </row>
-    <row r="120" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K120" s="24"/>
-      <c r="L120" s="24"/>
-      <c r="N120"/>
-      <c r="O120"/>
-    </row>
-    <row r="121" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="K121" s="24"/>
-      <c r="L121" s="24"/>
-      <c r="N121"/>
-      <c r="O121"/>
+    <row r="102" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D102" s="68"/>
+      <c r="E102" s="69"/>
+      <c r="F102" s="66"/>
+    </row>
+    <row r="103" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D103" s="70"/>
+      <c r="E103" s="71"/>
+      <c r="F103" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="55">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F13:F17"/>
+  <mergeCells count="38">
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="F83:F87"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F90:F92"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="F62:F64"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F67:F69"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="F76:F80"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F20:F24"/>
     <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F20:F24"/>
-    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F34:F38"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F41:F43"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F46:F50"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F53:F55"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F95:F99"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E103"/>
+    <mergeCell ref="F102:F103"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="F9:F10"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="D75:D79"/>
-    <mergeCell ref="H75:H79"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="F60:F62"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="F56:F57"/>
-    <mergeCell ref="F66:F68"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="H82:H86"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="B81:C81"/>
-    <mergeCell ref="B113:C114"/>
-    <mergeCell ref="D113:D114"/>
-    <mergeCell ref="F101:G102"/>
-    <mergeCell ref="H101:H102"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="D106:D110"/>
-    <mergeCell ref="D101:D103"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="H89:H91"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="D94:D98"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="F100:G100"/>
-    <mergeCell ref="F93:G93"/>
-    <mergeCell ref="F81:G81"/>
-    <mergeCell ref="F74:G74"/>
-    <mergeCell ref="H94:H98"/>
-    <mergeCell ref="D82:D86"/>
-    <mergeCell ref="F44:F48"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="F27:F31"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F13:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EF3BF063-FCC1-43B0-AFB1-C6F9111B94FE}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$B$4:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E4 E10 E57 C72:C73 G72:G73</xm:sqref>
+          <xm:sqref>E4 E10 E59 E73</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7C6B8CA4-BBDF-4720-83DB-EEB75CAAC296}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$B$10:$B$17</xm:f>
           </x14:formula1>
-          <xm:sqref>E14 E28 E45 C83 G83 C95 C107 G95 C76 G76</xm:sqref>
+          <xm:sqref>E14 E28 E35 E47 E84 E96</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{934B1DA1-8C91-4057-973F-82597951F8B7}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$F$5:$F$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D12:E12 D26:E26 D43:E43 B81:C81 F81:G81 B93:C93 B105:C105 F93:G93 B74:C74 F74:G74</xm:sqref>
+          <xm:sqref>D12:E12 D26:E26 D33:E33 D45:E45 D82:E82 D94:E94</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C1EA7122-9BB0-47F3-A320-6D1AE93FB4E0}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$D$10:$D$11</xm:f>
           </x14:formula1>
-          <xm:sqref>E17 E39 G79 C79 G98 C110 C98 G86 C86 E48 E31</xm:sqref>
+          <xm:sqref>E17 E31 E38 E50 E67 E87 E99</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6BE6F825-91BE-4CEC-9D14-5710077D0618}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$B$20:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>E15 C77 G96 C108 C96 G84 E29 E46 C84 G77</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F317EFE0-6C20-4FA6-8CE8-F5ABF95CC729}">
-          <x14:formula1>
-            <xm:f>'___Dropdown values'!$K$5:$K$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D33:E33 D50:E50 B88:C88 F88:G88 B100:C100</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{345D99D0-6529-4A67-8275-A029C65E5115}">
-          <x14:formula1>
-            <xm:f>'___Dropdown values'!$H$5:$H$6</xm:f>
-          </x14:formula1>
-          <xm:sqref>D59:E59</xm:sqref>
+          <xm:sqref>E15 E29 E36 E48 E85 E97</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{998DE1DC-BE8F-41C0-A011-BA46036902B2}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$G$5:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D19:E19</xm:sqref>
+          <xm:sqref>D19:E19 D75:E75</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{293526CA-88A8-463A-92FD-8CADF64CF4C1}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F9467DF0-84F4-4BD4-8755-0D48FDCB0007}">
+          <x14:formula1>
+            <xm:f>'___Dropdown values'!$K$5:$K$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D40:E40 D52:E52 D89:E89</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{45FFB53B-1ED2-49E5-B906-3156C5A5749B}">
+          <x14:formula1>
+            <xm:f>'___Dropdown values'!$D$4:$D$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E64</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86ECA534-E453-4537-BF1B-83AA46FFB5CD}">
+          <x14:formula1>
+            <xm:f>'___Dropdown values'!$H$5:$H$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>D61:E61</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0691EF2A-3318-4AFC-956C-54370E2E25A4}">
           <x14:formula1>
             <xm:f>'___Dropdown values'!$I$5:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D38:E38</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C124AD9A-B163-4E82-86EB-DE4F7DADE970}">
-          <x14:formula1>
-            <xm:f>'___Dropdown values'!$D$4:$D$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>E63</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D33A016A-FF6B-485D-892B-56B9C722EB80}">
-          <x14:formula1>
-            <xm:f>'___Dropdown values'!$D$4:$D$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>E62</xm:sqref>
+          <xm:sqref>D66:E66</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4510,7 +4150,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4519,16 +4159,16 @@
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -4536,7 +4176,7 @@
         <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
         <v>18</v>
@@ -4545,16 +4185,16 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="G1" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="H1" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -4574,14 +4214,11 @@
       <c r="E2">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>26</v>
       </c>
-      <c r="G2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
+      <c r="H2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4590,8 +4227,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B5" si="1">A3</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -4602,14 +4238,11 @@
       <c r="E3">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>25</v>
       </c>
-      <c r="G3" t="s">
-        <v>82</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
+      <c r="H3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4618,8 +4251,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
@@ -4630,14 +4262,8 @@
       <c r="E4">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
       <c r="G4" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4646,8 +4272,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -4658,54 +4283,18 @@
       <c r="E5">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="191" priority="264">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D3">
-    <cfRule type="expression" dxfId="190" priority="263">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="189" priority="262">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="188" priority="261">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="187" priority="260">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="expression" dxfId="186" priority="259">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
-    <cfRule type="expression" dxfId="185" priority="258">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="expression" dxfId="184" priority="257">
+    <cfRule type="expression" dxfId="185" priority="270">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:F2">
+    <cfRule type="expression" dxfId="184" priority="267">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4714,7 +4303,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
+  <conditionalFormatting sqref="E6:F6">
     <cfRule type="expression" dxfId="182" priority="255">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4724,27 +4313,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
+  <conditionalFormatting sqref="D8">
     <cfRule type="expression" dxfId="180" priority="253">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="D9">
     <cfRule type="expression" dxfId="179" priority="252">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
+  <conditionalFormatting sqref="E7:F7">
     <cfRule type="expression" dxfId="178" priority="251">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D9">
+  <conditionalFormatting sqref="E8:F8">
     <cfRule type="expression" dxfId="177" priority="250">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E9">
+  <conditionalFormatting sqref="E9:F9">
     <cfRule type="expression" dxfId="176" priority="249">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4754,27 +4343,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E10:F10">
+    <cfRule type="expression" dxfId="174" priority="247">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="expression" dxfId="174" priority="247">
+    <cfRule type="expression" dxfId="173" priority="246">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:F11">
+    <cfRule type="expression" dxfId="172" priority="245">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="expression" dxfId="173" priority="246">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="expression" dxfId="172" priority="245">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
     <cfRule type="expression" dxfId="171" priority="244">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
+  <conditionalFormatting sqref="E12:F12">
     <cfRule type="expression" dxfId="170" priority="243">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4784,7 +4373,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
+  <conditionalFormatting sqref="E13:F13">
     <cfRule type="expression" dxfId="168" priority="241">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4794,7 +4383,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
+  <conditionalFormatting sqref="E14:F14">
     <cfRule type="expression" dxfId="166" priority="239">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4804,27 +4393,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
+  <conditionalFormatting sqref="D16">
     <cfRule type="expression" dxfId="164" priority="237">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
+  <conditionalFormatting sqref="D17">
     <cfRule type="expression" dxfId="163" priority="236">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E16">
+  <conditionalFormatting sqref="E15:F15">
     <cfRule type="expression" dxfId="162" priority="235">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
+  <conditionalFormatting sqref="E16:F16">
     <cfRule type="expression" dxfId="161" priority="234">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
+  <conditionalFormatting sqref="E17:F17">
     <cfRule type="expression" dxfId="160" priority="233">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4834,27 +4423,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E18:F18">
+    <cfRule type="expression" dxfId="158" priority="231">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="158" priority="231">
+    <cfRule type="expression" dxfId="157" priority="230">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19:F19">
+    <cfRule type="expression" dxfId="156" priority="229">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="expression" dxfId="157" priority="230">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="156" priority="229">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
     <cfRule type="expression" dxfId="155" priority="228">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
+  <conditionalFormatting sqref="E20:F20">
     <cfRule type="expression" dxfId="154" priority="227">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4864,7 +4453,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
+  <conditionalFormatting sqref="E21:F21">
     <cfRule type="expression" dxfId="152" priority="225">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4874,7 +4463,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22">
+  <conditionalFormatting sqref="E22:F22">
     <cfRule type="expression" dxfId="150" priority="223">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4884,27 +4473,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
+  <conditionalFormatting sqref="D24">
     <cfRule type="expression" dxfId="148" priority="221">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
+  <conditionalFormatting sqref="D25">
     <cfRule type="expression" dxfId="147" priority="220">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E23:F23">
     <cfRule type="expression" dxfId="146" priority="219">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25">
+  <conditionalFormatting sqref="E24:F24">
     <cfRule type="expression" dxfId="145" priority="218">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
+  <conditionalFormatting sqref="E25:F25">
     <cfRule type="expression" dxfId="144" priority="217">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4914,27 +4503,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E26:F26">
+    <cfRule type="expression" dxfId="142" priority="215">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D27">
-    <cfRule type="expression" dxfId="142" priority="215">
+    <cfRule type="expression" dxfId="141" priority="214">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27:F27">
+    <cfRule type="expression" dxfId="140" priority="213">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28">
-    <cfRule type="expression" dxfId="141" priority="214">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="expression" dxfId="140" priority="213">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E27">
     <cfRule type="expression" dxfId="139" priority="212">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E28">
+  <conditionalFormatting sqref="E28:F28">
     <cfRule type="expression" dxfId="138" priority="211">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4944,7 +4533,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
+  <conditionalFormatting sqref="E29:F29">
     <cfRule type="expression" dxfId="136" priority="209">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4954,7 +4543,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E30">
+  <conditionalFormatting sqref="E30:F30">
     <cfRule type="expression" dxfId="134" priority="207">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4964,27 +4553,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E31">
+  <conditionalFormatting sqref="D32">
     <cfRule type="expression" dxfId="132" priority="205">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="D33">
     <cfRule type="expression" dxfId="131" priority="204">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E32">
+  <conditionalFormatting sqref="E31:F31">
     <cfRule type="expression" dxfId="130" priority="203">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33">
+  <conditionalFormatting sqref="E32:F32">
     <cfRule type="expression" dxfId="129" priority="202">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
+  <conditionalFormatting sqref="E33:F33">
     <cfRule type="expression" dxfId="128" priority="201">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -4994,27 +4583,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E34:F34">
+    <cfRule type="expression" dxfId="126" priority="199">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D35">
-    <cfRule type="expression" dxfId="126" priority="199">
+    <cfRule type="expression" dxfId="125" priority="198">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35:F35">
+    <cfRule type="expression" dxfId="124" priority="197">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="expression" dxfId="125" priority="198">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="124" priority="197">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
     <cfRule type="expression" dxfId="123" priority="196">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E36">
+  <conditionalFormatting sqref="E36:F36">
     <cfRule type="expression" dxfId="122" priority="195">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5024,7 +4613,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
+  <conditionalFormatting sqref="E37:F37">
     <cfRule type="expression" dxfId="120" priority="193">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5034,38 +4623,38 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
+  <conditionalFormatting sqref="E38:F38">
     <cfRule type="expression" dxfId="118" priority="191">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39">
-    <cfRule type="expression" dxfId="117" priority="190">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="116" priority="189">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40">
-    <cfRule type="expression" dxfId="115" priority="188">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E40">
-    <cfRule type="expression" dxfId="114" priority="187">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
-    <cfRule type="expression" dxfId="113" priority="186">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="112" priority="185">
+  <conditionalFormatting sqref="D71">
+    <cfRule type="expression" dxfId="117" priority="126">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D72">
+    <cfRule type="expression" dxfId="116" priority="125">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D73">
+    <cfRule type="expression" dxfId="115" priority="124">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E71:F71">
+    <cfRule type="expression" dxfId="114" priority="123">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E72:F72">
+    <cfRule type="expression" dxfId="113" priority="122">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E73:F73">
+    <cfRule type="expression" dxfId="112" priority="121">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5074,27 +4663,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E74:F74">
+    <cfRule type="expression" dxfId="110" priority="119">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="expression" dxfId="110" priority="119">
+    <cfRule type="expression" dxfId="109" priority="118">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E75:F75">
+    <cfRule type="expression" dxfId="108" priority="117">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="expression" dxfId="109" priority="118">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E74">
-    <cfRule type="expression" dxfId="108" priority="117">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E75">
     <cfRule type="expression" dxfId="107" priority="116">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E76">
+  <conditionalFormatting sqref="E76:F76">
     <cfRule type="expression" dxfId="106" priority="115">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5104,7 +4693,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E77">
+  <conditionalFormatting sqref="E77:F77">
     <cfRule type="expression" dxfId="104" priority="113">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5114,7 +4703,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E78">
+  <conditionalFormatting sqref="E78:F78">
     <cfRule type="expression" dxfId="102" priority="111">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5124,27 +4713,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E79">
+  <conditionalFormatting sqref="D80">
     <cfRule type="expression" dxfId="100" priority="109">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D80">
+  <conditionalFormatting sqref="D81">
     <cfRule type="expression" dxfId="99" priority="108">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E80">
+  <conditionalFormatting sqref="E79:F79">
     <cfRule type="expression" dxfId="98" priority="107">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D81">
+  <conditionalFormatting sqref="E80:F80">
     <cfRule type="expression" dxfId="97" priority="106">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E81">
+  <conditionalFormatting sqref="E81:F81">
     <cfRule type="expression" dxfId="96" priority="105">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5154,27 +4743,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E82:F82">
+    <cfRule type="expression" dxfId="94" priority="103">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D83">
-    <cfRule type="expression" dxfId="94" priority="103">
+    <cfRule type="expression" dxfId="93" priority="102">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E83:F83">
+    <cfRule type="expression" dxfId="92" priority="101">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D84">
-    <cfRule type="expression" dxfId="93" priority="102">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E82">
-    <cfRule type="expression" dxfId="92" priority="101">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E83">
     <cfRule type="expression" dxfId="91" priority="100">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84">
+  <conditionalFormatting sqref="E84:F84">
     <cfRule type="expression" dxfId="90" priority="99">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5184,7 +4773,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E85">
+  <conditionalFormatting sqref="E85:F85">
     <cfRule type="expression" dxfId="88" priority="97">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5194,7 +4783,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E86">
+  <conditionalFormatting sqref="E86:F86">
     <cfRule type="expression" dxfId="86" priority="95">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5204,27 +4793,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87">
+  <conditionalFormatting sqref="D88">
     <cfRule type="expression" dxfId="84" priority="93">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D88">
+  <conditionalFormatting sqref="D89">
     <cfRule type="expression" dxfId="83" priority="92">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E88">
+  <conditionalFormatting sqref="E87:F87">
     <cfRule type="expression" dxfId="82" priority="91">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D89">
+  <conditionalFormatting sqref="E88:F88">
     <cfRule type="expression" dxfId="81" priority="90">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E89">
+  <conditionalFormatting sqref="E89:F89">
     <cfRule type="expression" dxfId="80" priority="89">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5234,27 +4823,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E90:F90">
+    <cfRule type="expression" dxfId="78" priority="87">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D91">
-    <cfRule type="expression" dxfId="78" priority="87">
+    <cfRule type="expression" dxfId="77" priority="86">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E91:F91">
+    <cfRule type="expression" dxfId="76" priority="85">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="expression" dxfId="77" priority="86">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E90">
-    <cfRule type="expression" dxfId="76" priority="85">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E91">
     <cfRule type="expression" dxfId="75" priority="84">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
+  <conditionalFormatting sqref="E92:F92">
     <cfRule type="expression" dxfId="74" priority="83">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5264,7 +4853,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E93">
+  <conditionalFormatting sqref="E93:F93">
     <cfRule type="expression" dxfId="72" priority="81">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5274,37 +4863,37 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E94">
+  <conditionalFormatting sqref="E94:F94">
     <cfRule type="expression" dxfId="70" priority="79">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D95">
+  <conditionalFormatting sqref="D39">
     <cfRule type="expression" dxfId="69" priority="78">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E95">
+  <conditionalFormatting sqref="D40">
     <cfRule type="expression" dxfId="68" priority="77">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D96">
+  <conditionalFormatting sqref="D41">
     <cfRule type="expression" dxfId="67" priority="76">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E96">
+  <conditionalFormatting sqref="E39:F39">
     <cfRule type="expression" dxfId="66" priority="75">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D97">
+  <conditionalFormatting sqref="E40:F40">
     <cfRule type="expression" dxfId="65" priority="74">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E97">
+  <conditionalFormatting sqref="E41:F41">
     <cfRule type="expression" dxfId="64" priority="73">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5314,38 +4903,38 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D43">
+  <conditionalFormatting sqref="E42:F42">
     <cfRule type="expression" dxfId="62" priority="71">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="61" priority="70">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E42">
-    <cfRule type="expression" dxfId="60" priority="69">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E43">
-    <cfRule type="expression" dxfId="59" priority="68">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="58" priority="67">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45">
-    <cfRule type="expression" dxfId="57" priority="66">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="expression" dxfId="56" priority="65">
+  <conditionalFormatting sqref="D47">
+    <cfRule type="expression" dxfId="61" priority="62">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="expression" dxfId="60" priority="61">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49">
+    <cfRule type="expression" dxfId="59" priority="60">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:F47">
+    <cfRule type="expression" dxfId="58" priority="59">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48:F48">
+    <cfRule type="expression" dxfId="57" priority="58">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49:F49">
+    <cfRule type="expression" dxfId="56" priority="57">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5354,27 +4943,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E50:F50">
+    <cfRule type="expression" dxfId="54" priority="55">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="54" priority="55">
+    <cfRule type="expression" dxfId="53" priority="54">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51:F51">
+    <cfRule type="expression" dxfId="52" priority="53">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="expression" dxfId="53" priority="54">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E50">
-    <cfRule type="expression" dxfId="52" priority="53">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
     <cfRule type="expression" dxfId="51" priority="52">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
+  <conditionalFormatting sqref="E52:F52">
     <cfRule type="expression" dxfId="50" priority="51">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5384,7 +4973,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E53">
+  <conditionalFormatting sqref="E53:F53">
     <cfRule type="expression" dxfId="48" priority="49">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5394,7 +4983,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E54">
+  <conditionalFormatting sqref="E54:F54">
     <cfRule type="expression" dxfId="46" priority="47">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5404,27 +4993,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E55">
+  <conditionalFormatting sqref="D56">
     <cfRule type="expression" dxfId="44" priority="45">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56">
+  <conditionalFormatting sqref="D57">
     <cfRule type="expression" dxfId="43" priority="44">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56">
+  <conditionalFormatting sqref="E55:F55">
     <cfRule type="expression" dxfId="42" priority="43">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D57">
+  <conditionalFormatting sqref="E56:F56">
     <cfRule type="expression" dxfId="41" priority="42">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E57">
+  <conditionalFormatting sqref="E57:F57">
     <cfRule type="expression" dxfId="40" priority="41">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5434,27 +5023,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E58:F58">
+    <cfRule type="expression" dxfId="38" priority="39">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="38" priority="39">
+    <cfRule type="expression" dxfId="37" priority="38">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59:F59">
+    <cfRule type="expression" dxfId="36" priority="37">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="37" priority="38">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
-    <cfRule type="expression" dxfId="36" priority="37">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
     <cfRule type="expression" dxfId="35" priority="36">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E60">
+  <conditionalFormatting sqref="E60:F60">
     <cfRule type="expression" dxfId="34" priority="35">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5464,7 +5053,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E61">
+  <conditionalFormatting sqref="E61:F61">
     <cfRule type="expression" dxfId="32" priority="33">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5474,7 +5063,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E62">
+  <conditionalFormatting sqref="E62:F62">
     <cfRule type="expression" dxfId="30" priority="31">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5484,27 +5073,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
+  <conditionalFormatting sqref="D64">
     <cfRule type="expression" dxfId="28" priority="29">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="D65">
     <cfRule type="expression" dxfId="27" priority="28">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
+  <conditionalFormatting sqref="E63:F63">
     <cfRule type="expression" dxfId="26" priority="27">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="E64:F64">
     <cfRule type="expression" dxfId="25" priority="26">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
+  <conditionalFormatting sqref="E65:F65">
     <cfRule type="expression" dxfId="24" priority="25">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5514,27 +5103,27 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E66:F66">
+    <cfRule type="expression" dxfId="22" priority="23">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D67">
-    <cfRule type="expression" dxfId="22" priority="23">
+    <cfRule type="expression" dxfId="21" priority="22">
+      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67:F67">
+    <cfRule type="expression" dxfId="20" priority="21">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68">
-    <cfRule type="expression" dxfId="21" priority="22">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="expression" dxfId="20" priority="21">
-      <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
     <cfRule type="expression" dxfId="19" priority="20">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
+  <conditionalFormatting sqref="E68:F68">
     <cfRule type="expression" dxfId="18" priority="19">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5544,7 +5133,7 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
+  <conditionalFormatting sqref="E69:F69">
     <cfRule type="expression" dxfId="16" priority="17">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5554,37 +5143,37 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E70">
+  <conditionalFormatting sqref="E70:F70">
     <cfRule type="expression" dxfId="14" priority="15">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D71">
+  <conditionalFormatting sqref="D43">
     <cfRule type="expression" dxfId="13" priority="14">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E71">
+  <conditionalFormatting sqref="E43:F43">
     <cfRule type="expression" dxfId="12" priority="13">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D72">
+  <conditionalFormatting sqref="D44">
     <cfRule type="expression" dxfId="11" priority="12">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E72">
+  <conditionalFormatting sqref="E44:F44">
     <cfRule type="expression" dxfId="10" priority="11">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D73">
+  <conditionalFormatting sqref="D45">
     <cfRule type="expression" dxfId="9" priority="10">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E73">
+  <conditionalFormatting sqref="E45:F45">
     <cfRule type="expression" dxfId="8" priority="9">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5594,37 +5183,37 @@
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E46">
+  <conditionalFormatting sqref="E46:F46">
     <cfRule type="expression" dxfId="6" priority="7">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
+  <conditionalFormatting sqref="D3">
     <cfRule type="expression" dxfId="5" priority="6">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E47">
+  <conditionalFormatting sqref="E3:F3">
     <cfRule type="expression" dxfId="4" priority="5">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D48">
+  <conditionalFormatting sqref="D4">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E48">
+  <conditionalFormatting sqref="E4:F4">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49">
+  <conditionalFormatting sqref="D5">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E49">
+  <conditionalFormatting sqref="E5:F5">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>IF($D$2&lt;10,TRUE,IF($D$2&gt;50,TRUE,FALSE))</formula>
     </cfRule>
@@ -5858,18 +5447,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5892,18 +5481,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158388FD-FCB9-4D40-8807-AFB22AE8C172}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46E792D2-13D9-445F-AE7B-CF179A33399C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{158388FD-FCB9-4D40-8807-AFB22AE8C172}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>